<commit_message>
Did not finish the gw winner function
</commit_message>
<xml_diff>
--- a/FPL Luster totaloversikt.xlsx
+++ b/FPL Luster totaloversikt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\FantasyLeaguePointsFetcher\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4043B8DA-5374-497E-BF07-F012CC289148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7CE8C4B-9A46-4A0D-A86C-5010D4CA27DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51390" yWindow="2040" windowWidth="38610" windowHeight="15345" activeTab="2" xr2:uid="{9393CECB-8678-4F9E-A49E-EF671E63BC0A}"/>
+    <workbookView xWindow="51810" yWindow="1920" windowWidth="30030" windowHeight="14280" activeTab="2" xr2:uid="{9393CECB-8678-4F9E-A49E-EF671E63BC0A}"/>
   </bookViews>
   <sheets>
     <sheet name="GW oversikt" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="First_Day">Seiersoversikt!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1" fullPrecision="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="183">
   <si>
     <t>Luster FPL oversikt</t>
   </si>
@@ -597,7 +597,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -805,57 +806,54 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="12" applyFont="1" fillId="4" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0"/>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="12" applyFont="1" fillId="5" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0"/>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="13" applyFont="1" fillId="3" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0"/>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="2" applyFont="1" fillId="0" applyFill="0" borderId="3" applyBorder="1" applyProtection="0" applyAlignment="0"/>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="3" applyFont="1" fillId="0" applyFill="0" borderId="4" applyBorder="1" applyProtection="0" applyAlignment="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" fontId="1" applyFont="1" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" applyFont="1" fillId="0" borderId="1" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" fontId="1" applyFont="1" fillId="0" borderId="2" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" fontId="5" applyFont="1" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" applyFont="1" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" applyFont="1" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" applyFont="1" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" applyFont="1" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" applyFont="1" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="10" applyFont="1" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="11" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" fontId="11" applyFont="1" fillId="2" applyFill="1" borderId="2" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" fontId="12" applyFont="1" fillId="4" applyFill="1" borderId="5" applyBorder="1" xfId="1"/>
+    <xf numFmtId="0" fontId="0" applyFont="1" fillId="4" applyFill="1" borderId="5" applyBorder="1" xfId="1"/>
+    <xf numFmtId="0" fontId="13" applyFont="1" fillId="3" applyFill="1" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="12" applyFont="1" fillId="5" applyFill="1" borderId="5" applyBorder="1" xfId="2" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" applyFont="1" fillId="5" applyFill="1" borderId="5" applyBorder="1" xfId="2"/>
+    <xf numFmtId="0" fontId="0" applyFont="1" fillId="5" applyFill="1" borderId="5" applyBorder="1" xfId="2" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="5"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" applyFont="1" fillId="0" borderId="4" applyBorder="1" xfId="5"/>
+    <xf numFmtId="0" fontId="14" applyFont="1" fillId="0" borderId="0" applyBorder="1" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" applyFont="1" fillId="0" borderId="6" applyBorder="1" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="4" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" applyFont="1" fillId="0" borderId="3" applyBorder="1" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" applyFont="1" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="20 % – uthevingsfarge 1" xfId="1" builtinId="30"/>
@@ -954,20 +952,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E90C81C4-95FC-4A01-A65E-58F76846EE81}" name="Tabell4" displayName="Tabell4" ref="A3:I28" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E90C81C4-95FC-4A01-A65E-58F76846EE81}" name="Tabell4" displayName="Tabell4" ref="A3:I28" totalsRowShown="0" headerRowDxfId="2" dataDxfId="2">
   <autoFilter ref="A3:I28" xr:uid="{E90C81C4-95FC-4A01-A65E-58F76846EE81}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:I28">
     <sortCondition ref="B3:B28"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{9A32B1F6-F8CB-4699-B624-42469B8910F7}" name="Lagnamn" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{DF6D108C-113A-4799-B990-BC2C37720997}" name="Deltakar" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{9A32B1F6-F8CB-4699-B624-42469B8910F7}" name="Lagnamn" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{DF6D108C-113A-4799-B990-BC2C37720997}" name="Deltakar" dataDxfId="2"/>
     <tableColumn id="9" xr3:uid="{1BE17DC9-CEDA-4780-B5B9-6D2F30F3FC1E}" name="Betalt" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{C054776D-FB3B-43E4-8E3D-15A57D0CA136}" name="Rundersigera" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{B81FCAF0-57D4-419D-A6AB-2A6EF7DAF000}" name="Månadens manager" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{9D7A61DE-D7DD-449F-9053-3A41D3A70376}" name="Julecup rundesigera" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{7C2101C8-0F07-40C0-BFA8-CC10D84097B5}" name="Julecup siger" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{58C925C2-F94A-4295-B305-0F04D789387E}" name="Vinnar halvspelt" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{C054776D-FB3B-43E4-8E3D-15A57D0CA136}" name="Rundersigera" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{B81FCAF0-57D4-419D-A6AB-2A6EF7DAF000}" name="Månadens manager" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{9D7A61DE-D7DD-449F-9053-3A41D3A70376}" name="Julecup rundesigera" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{7C2101C8-0F07-40C0-BFA8-CC10D84097B5}" name="Julecup siger" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{58C925C2-F94A-4295-B305-0F04D789387E}" name="Vinnar halvspelt" dataDxfId="2"/>
     <tableColumn id="8" xr3:uid="{D494F2BF-B492-46A7-B9C3-DC48C800A910}" name="Kolonne1" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -981,7 +979,7 @@
     <sortCondition ref="B3:B27"/>
   </sortState>
   <tableColumns count="40">
-    <tableColumn id="1" xr3:uid="{74CEA007-FA61-3D40-A38E-5915AED44115}" name="Lagnamn" dataDxfId="1" dataCellStyle="Totalt"/>
+    <tableColumn id="1" xr3:uid="{74CEA007-FA61-3D40-A38E-5915AED44115}" name="Lagnamn" dataDxfId="0" dataCellStyle="Totalt"/>
     <tableColumn id="2" xr3:uid="{EB31D824-E353-F34A-AC67-139C8D0DCF1B}" name="Deltakar" dataDxfId="0" dataCellStyle="Totalt"/>
     <tableColumn id="3" xr3:uid="{07467C74-1A1C-614D-8DD7-DEF2929F0147}" name="GW1"/>
     <tableColumn id="4" xr3:uid="{905EED4D-BAD6-814F-80FA-B0DF9447BB4F}" name="GW2"/>
@@ -1351,29 +1349,29 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="1" width="25.140625" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="23.7109375" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" bestFit="1" width="6.42578125" customWidth="1"/>
+    <col min="5" max="5" bestFit="1" width="18.42578125" customWidth="1"/>
     <col min="6" max="6" width="19.140625" customWidth="1"/>
     <col min="7" max="7" width="16.85546875" customWidth="1"/>
-    <col min="8" max="8" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="23" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="27" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" bestFit="1" width="20.42578125" customWidth="1"/>
+    <col min="9" max="9" bestFit="1" width="23" customWidth="1"/>
+    <col min="10" max="11" bestFit="1" width="20.42578125" customWidth="1"/>
+    <col min="12" max="12" bestFit="1" width="23" customWidth="1"/>
+    <col min="13" max="13" bestFit="1" width="35.42578125" customWidth="1"/>
+    <col min="14" max="23" bestFit="1" width="3.7109375" customWidth="1"/>
+    <col min="24" max="24" bestFit="1" width="5.42578125" customWidth="1"/>
+    <col min="25" max="27" bestFit="1" width="3.7109375" customWidth="1"/>
+    <col min="28" max="28" bestFit="1" width="6.85546875" customWidth="1"/>
+    <col min="29" max="29" bestFit="1" width="5.42578125" customWidth="1"/>
+    <col min="30" max="30" bestFit="1" width="3.7109375" customWidth="1"/>
+    <col min="31" max="31" bestFit="1" width="6.85546875" customWidth="1"/>
+    <col min="32" max="33" bestFit="1" width="3.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" ht="15" customHeight="1">
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
@@ -1385,7 +1383,7 @@
       <c r="G1" s="21"/>
       <c r="H1" s="21"/>
     </row>
-    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" ht="15" customHeight="1">
       <c r="A2" s="22"/>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
@@ -1395,7 +1393,7 @@
       <c r="G2" s="22"/>
       <c r="H2" s="22"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3">
       <c r="A3" s="14" t="s">
         <v>1</v>
       </c>
@@ -1427,7 +1425,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4">
       <c r="A4" s="14" t="s">
         <v>11</v>
       </c>
@@ -1447,7 +1445,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5">
       <c r="A5" s="14" t="s">
         <v>15</v>
       </c>
@@ -1467,7 +1465,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6">
       <c r="A6" s="14" t="s">
         <v>19</v>
       </c>
@@ -1487,7 +1485,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7">
       <c r="A7" s="18"/>
       <c r="B7" s="18"/>
       <c r="C7" s="17"/>
@@ -1505,7 +1503,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8">
       <c r="A8" s="14" t="s">
         <v>26</v>
       </c>
@@ -1525,7 +1523,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9">
       <c r="A9" s="14" t="s">
         <v>30</v>
       </c>
@@ -1545,7 +1543,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10">
       <c r="A10" s="14" t="s">
         <v>34</v>
       </c>
@@ -1565,7 +1563,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11">
       <c r="A11" s="18"/>
       <c r="B11" s="18"/>
       <c r="C11" s="17"/>
@@ -1583,7 +1581,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12">
       <c r="A12" s="14" t="s">
         <v>41</v>
       </c>
@@ -1603,7 +1601,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13">
       <c r="A13" s="14" t="s">
         <v>45</v>
       </c>
@@ -1623,7 +1621,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14">
       <c r="A14" s="14" t="s">
         <v>49</v>
       </c>
@@ -1643,7 +1641,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15">
       <c r="A15" s="18"/>
       <c r="B15" s="18"/>
       <c r="C15" s="17"/>
@@ -1661,7 +1659,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16">
       <c r="A16" s="14" t="s">
         <v>56</v>
       </c>
@@ -1681,7 +1679,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17">
       <c r="A17" s="14" t="s">
         <v>60</v>
       </c>
@@ -1701,7 +1699,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18">
       <c r="A18" s="14" t="s">
         <v>64</v>
       </c>
@@ -1721,7 +1719,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19">
       <c r="A19" s="14" t="s">
         <v>68</v>
       </c>
@@ -1741,7 +1739,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20">
       <c r="A20" s="18"/>
       <c r="B20" s="18"/>
       <c r="C20" s="17"/>
@@ -1759,7 +1757,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21">
       <c r="A21" s="14" t="s">
         <v>75</v>
       </c>
@@ -1779,7 +1777,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22">
       <c r="A22" s="14" t="s">
         <v>79</v>
       </c>
@@ -1799,7 +1797,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23">
       <c r="A23" s="14" t="s">
         <v>83</v>
       </c>
@@ -1819,7 +1817,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24">
       <c r="A24" s="14" t="s">
         <v>87</v>
       </c>
@@ -1841,7 +1839,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25">
       <c r="A25" s="14" t="s">
         <v>92</v>
       </c>
@@ -1863,7 +1861,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26">
       <c r="A26" s="14" t="s">
         <v>96</v>
       </c>
@@ -1885,7 +1883,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27">
       <c r="A27" s="18"/>
       <c r="B27" s="18"/>
       <c r="C27" s="17"/>
@@ -1905,7 +1903,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28">
       <c r="A28" s="14" t="s">
         <v>104</v>
       </c>
@@ -1919,7 +1917,7 @@
       <c r="G28" s="14"/>
       <c r="H28" s="14"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29">
       <c r="A29" s="14" t="s">
         <v>106</v>
       </c>
@@ -1933,7 +1931,7 @@
       <c r="G29" s="14"/>
       <c r="H29" s="14"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30">
       <c r="A30" s="14" t="s">
         <v>108</v>
       </c>
@@ -1947,7 +1945,7 @@
       <c r="G30" s="14"/>
       <c r="H30" s="14"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31">
       <c r="A31" s="14" t="s">
         <v>110</v>
       </c>
@@ -1961,7 +1959,7 @@
       <c r="G31" s="14"/>
       <c r="H31" s="14"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32">
       <c r="A32" s="18"/>
       <c r="B32" s="18"/>
       <c r="C32" s="18"/>
@@ -1973,7 +1971,7 @@
       <c r="G32" s="18"/>
       <c r="H32" s="18"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33">
       <c r="A33" s="14" t="s">
         <v>113</v>
       </c>
@@ -1987,7 +1985,7 @@
       <c r="G33" s="14"/>
       <c r="H33" s="14"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34">
       <c r="A34" s="14" t="s">
         <v>115</v>
       </c>
@@ -2001,7 +1999,7 @@
       <c r="G34" s="14"/>
       <c r="H34" s="14"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35">
       <c r="A35" s="14" t="s">
         <v>117</v>
       </c>
@@ -2015,7 +2013,7 @@
       <c r="G35" s="14"/>
       <c r="H35" s="14"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36">
       <c r="A36" s="14" t="s">
         <v>119</v>
       </c>
@@ -2029,7 +2027,7 @@
       <c r="G36" s="14"/>
       <c r="H36" s="14"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37">
       <c r="A37" s="18"/>
       <c r="B37" s="18"/>
       <c r="C37" s="18"/>
@@ -2041,7 +2039,7 @@
       <c r="G37" s="18"/>
       <c r="H37" s="18"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38">
       <c r="A38" s="14" t="s">
         <v>122</v>
       </c>
@@ -2055,7 +2053,7 @@
       <c r="G38" s="14"/>
       <c r="H38" s="14"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39">
       <c r="A39" s="14" t="s">
         <v>124</v>
       </c>
@@ -2069,7 +2067,7 @@
       <c r="G39" s="14"/>
       <c r="H39" s="14"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40">
       <c r="A40" s="18"/>
       <c r="B40" s="18"/>
       <c r="C40" s="18"/>
@@ -2081,7 +2079,7 @@
       <c r="G40" s="18"/>
       <c r="H40" s="18"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41">
       <c r="A41" s="14" t="s">
         <v>127</v>
       </c>
@@ -2095,7 +2093,7 @@
       <c r="G41" s="14"/>
       <c r="H41" s="14"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42">
       <c r="A42" s="14" t="s">
         <v>129</v>
       </c>
@@ -2109,7 +2107,7 @@
       <c r="G42" s="14"/>
       <c r="H42" s="14"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43">
       <c r="A43" s="14" t="s">
         <v>131</v>
       </c>
@@ -2123,7 +2121,7 @@
       <c r="G43" s="14"/>
       <c r="H43" s="14"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44">
       <c r="A44" s="14" t="s">
         <v>133</v>
       </c>
@@ -2137,7 +2135,7 @@
       <c r="G44" s="14"/>
       <c r="H44" s="14"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45">
       <c r="A45" s="14" t="s">
         <v>135</v>
       </c>
@@ -2151,7 +2149,7 @@
       <c r="G45" s="14"/>
       <c r="H45" s="14"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46">
       <c r="A46" s="18"/>
       <c r="B46" s="18"/>
       <c r="C46" s="18"/>
@@ -2163,7 +2161,7 @@
       <c r="G46" s="18"/>
       <c r="H46" s="18"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47">
       <c r="A47" s="14" t="s">
         <v>138</v>
       </c>
@@ -2177,7 +2175,7 @@
       <c r="G47" s="14"/>
       <c r="H47" s="14"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48">
       <c r="A48" s="14" t="s">
         <v>140</v>
       </c>
@@ -2191,7 +2189,7 @@
       <c r="G48" s="14"/>
       <c r="H48" s="14"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49">
       <c r="A49" s="14" t="s">
         <v>142</v>
       </c>
@@ -2205,7 +2203,7 @@
       <c r="G49" s="14"/>
       <c r="H49" s="14"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50">
       <c r="A50" s="14" t="s">
         <v>144</v>
       </c>
@@ -2219,7 +2217,7 @@
       <c r="G50" s="14"/>
       <c r="H50" s="14"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51">
       <c r="A51" s="18"/>
       <c r="B51" s="18"/>
       <c r="C51" s="18"/>
@@ -2232,11 +2230,12 @@
       <c r="H51" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells>
     <mergeCell ref="A1:H2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
@@ -2251,17 +2250,17 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="1" width="22" customWidth="1"/>
+    <col min="3" max="3" bestFit="1" width="8.42578125" customWidth="1"/>
+    <col min="4" max="4" bestFit="1" width="20.42578125" customWidth="1"/>
+    <col min="5" max="5" bestFit="1" width="19.85546875" customWidth="1"/>
+    <col min="6" max="6" bestFit="1" width="20.140625" customWidth="1"/>
+    <col min="7" max="7" bestFit="1" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" bestFit="1" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" bestFit="1" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" s="23" t="s">
         <v>147</v>
       </c>
@@ -2274,7 +2273,7 @@
       <c r="H1" s="23"/>
       <c r="I1" s="23"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2">
       <c r="A2" s="23"/>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
@@ -2285,7 +2284,7 @@
       <c r="H2" s="23"/>
       <c r="I2" s="23"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -2314,7 +2313,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4">
       <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
@@ -2331,7 +2330,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
@@ -2348,7 +2347,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
@@ -2365,7 +2364,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7">
       <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
@@ -2382,7 +2381,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8">
       <c r="A8" s="2" t="s">
         <v>28</v>
       </c>
@@ -2399,7 +2398,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9">
       <c r="A9" s="2" t="s">
         <v>32</v>
       </c>
@@ -2416,7 +2415,7 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10">
       <c r="A10" s="2" t="s">
         <v>36</v>
       </c>
@@ -2433,7 +2432,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11">
       <c r="A11" s="2" t="s">
         <v>39</v>
       </c>
@@ -2450,7 +2449,7 @@
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12">
       <c r="A12" s="2" t="s">
         <v>43</v>
       </c>
@@ -2467,7 +2466,7 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13">
       <c r="A13" s="2" t="s">
         <v>47</v>
       </c>
@@ -2484,7 +2483,7 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14">
       <c r="A14" s="2" t="s">
         <v>51</v>
       </c>
@@ -2501,7 +2500,7 @@
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15">
       <c r="A15" s="2" t="s">
         <v>54</v>
       </c>
@@ -2518,7 +2517,7 @@
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16">
       <c r="A16" s="2" t="s">
         <v>58</v>
       </c>
@@ -2535,7 +2534,7 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17">
       <c r="A17" s="2" t="s">
         <v>62</v>
       </c>
@@ -2552,7 +2551,7 @@
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18">
       <c r="A18" s="2" t="s">
         <v>66</v>
       </c>
@@ -2569,7 +2568,7 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19">
       <c r="A19" s="2" t="s">
         <v>70</v>
       </c>
@@ -2586,7 +2585,7 @@
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20">
       <c r="A20" s="2" t="s">
         <v>73</v>
       </c>
@@ -2603,7 +2602,7 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21">
       <c r="A21" s="2" t="s">
         <v>77</v>
       </c>
@@ -2620,7 +2619,7 @@
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22">
       <c r="A22" s="2" t="s">
         <v>81</v>
       </c>
@@ -2637,7 +2636,7 @@
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23">
       <c r="A23" s="2" t="s">
         <v>85</v>
       </c>
@@ -2654,7 +2653,7 @@
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24">
       <c r="A24" s="2" t="s">
         <v>90</v>
       </c>
@@ -2671,7 +2670,7 @@
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25">
       <c r="A25" s="2" t="s">
         <v>94</v>
       </c>
@@ -2687,7 +2686,7 @@
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26">
       <c r="A26" s="2" t="s">
         <v>98</v>
       </c>
@@ -2703,7 +2702,7 @@
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27">
       <c r="A27" s="2" t="s">
         <v>102</v>
       </c>
@@ -2720,7 +2719,7 @@
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -2735,11 +2734,12 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D4:D24">
     <sortCondition ref="D4:D24"/>
   </sortState>
-  <mergeCells count="1">
+  <mergeCells>
     <mergeCell ref="A1:I2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -2751,16 +2751,16 @@
   <dimension ref="A1:AN27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="1" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" bestFit="1" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" s="21" t="s">
         <v>156</v>
       </c>
@@ -2771,7 +2771,7 @@
       <c r="F1" s="21"/>
       <c r="G1" s="21"/>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="2">
       <c r="A2" s="22"/>
       <c r="B2" s="22"/>
       <c r="C2" s="22"/>
@@ -2780,471 +2780,472 @@
       <c r="F2" s="22"/>
       <c r="G2" s="22"/>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+    <row r="3">
+      <c r="A3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="O3" t="s">
+      <c r="O3" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="P3" t="s">
+      <c r="P3" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="Q3" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="R3" t="s">
+      <c r="R3" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="S3" t="s">
+      <c r="S3" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="T3" t="s">
+      <c r="T3" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="U3" t="s">
+      <c r="U3" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="V3" t="s">
+      <c r="V3" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="W3" t="s">
+      <c r="W3" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="X3" t="s">
+      <c r="X3" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Y3" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="Z3" s="0" t="s">
         <v>114</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AA3" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AB3" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AC3" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AD3" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AE3" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="AF3" t="s">
+      <c r="AF3" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="AG3" t="s">
+      <c r="AG3" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="AH3" t="s">
+      <c r="AH3" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="AI3" t="s">
+      <c r="AI3" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="AJ3" t="s">
+      <c r="AJ3" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="AK3" t="s">
+      <c r="AK3" s="0" t="s">
         <v>139</v>
       </c>
-      <c r="AL3" t="s">
+      <c r="AL3" s="0" t="s">
         <v>141</v>
       </c>
-      <c r="AM3" t="s">
+      <c r="AM3" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="AN3" t="s">
+      <c r="AN3" s="0" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+    <row r="4">
+      <c r="A4" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="0">
         <v>67</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="0">
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
+    <row r="5">
+      <c r="A5" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="0">
         <v>61</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="0">
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
+    <row r="6">
+      <c r="A6" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="0">
         <v>69</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="0">
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
+    <row r="7">
+      <c r="A7" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="0">
         <v>70</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="0">
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A8" s="27" t="s">
+    <row r="8">
+      <c r="A8" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="0">
         <v>75</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="0">
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A9" s="27" t="s">
+    <row r="9">
+      <c r="A9" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="0">
         <v>45</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="0">
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A10" s="27" t="s">
+    <row r="10">
+      <c r="A10" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="0">
         <v>64</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="0">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A11" s="27" t="s">
+    <row r="11">
+      <c r="A11" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="0">
         <v>67</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="0">
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
+    <row r="12">
+      <c r="A12" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="0">
         <v>48</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="0">
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A13" s="27" t="s">
+    <row r="13">
+      <c r="A13" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="0">
         <v>57</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="0">
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A14" s="27" t="s">
+    <row r="14">
+      <c r="A14" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="0">
         <v>84</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="0">
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A15" s="27" t="s">
+    <row r="15">
+      <c r="A15" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="0">
         <v>55</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="0">
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A16" s="27" t="s">
+    <row r="16">
+      <c r="A16" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="0">
         <v>75</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="0">
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="27" t="s">
+    <row r="17">
+      <c r="A17" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="B17" s="27" t="s">
+      <c r="B17" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="0">
         <v>79</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="0">
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="27" t="s">
+    <row r="18">
+      <c r="A18" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="0">
         <v>53</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="0">
         <v>73</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="27" t="s">
+    <row r="19">
+      <c r="A19" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="0">
         <v>68</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="0">
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="27" t="s">
+    <row r="20">
+      <c r="A20" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="B20" s="27" t="s">
+      <c r="B20" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="0">
         <v>76</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="0">
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="27" t="s">
+    <row r="21">
+      <c r="A21" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="B21" s="27" t="s">
+      <c r="B21" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="0">
         <v>42</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="0">
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="27" t="s">
+    <row r="22">
+      <c r="A22" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="B22" s="27" t="s">
+      <c r="B22" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="0">
         <v>81</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="0">
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="27" t="s">
+    <row r="23">
+      <c r="A23" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="B23" s="27" t="s">
+      <c r="B23" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="0">
         <v>72</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="0">
         <v>77</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="27" t="s">
+    <row r="24">
+      <c r="A24" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="B24" s="27" t="s">
+      <c r="B24" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="0">
         <v>62</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="0">
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="27" t="s">
+    <row r="25">
+      <c r="A25" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="B25" s="27" t="s">
+      <c r="B25" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="0">
         <v>54</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="0">
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="27" t="s">
+    <row r="26">
+      <c r="A26" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="B26" s="27" t="s">
+      <c r="B26" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="0">
         <v>48</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="0">
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="27" t="s">
+    <row r="27">
+      <c r="A27" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="B27" s="27" t="s">
+      <c r="B27" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="0">
         <v>60</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="0">
         <v>81</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells>
     <mergeCell ref="A1:G2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0"/>
+  <headerFooter/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -3262,10 +3263,10 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.140625" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" bestFit="1" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" s="23" t="s">
         <v>157</v>
       </c>
@@ -3274,147 +3275,147 @@
       <c r="D1" s="23"/>
       <c r="E1" s="23"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2">
       <c r="A2" s="23"/>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3">
+      <c r="A3" s="0" t="s">
         <v>158</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="0" t="s">
         <v>161</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="0">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4">
       <c r="A4" s="5" t="s">
         <v>162</v>
       </c>
       <c r="B4" s="7">
         <v>125</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="0">
         <f>B4*F3</f>
         <v>4750</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="0" t="s">
         <v>163</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="0">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5">
       <c r="A5" s="5" t="s">
         <v>164</v>
       </c>
       <c r="B5" s="7">
         <v>250</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="0">
         <f>B5*F4</f>
         <v>2500</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="0" t="s">
         <v>165</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="0">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" ht="30">
       <c r="A6" s="5" t="s">
         <v>166</v>
       </c>
       <c r="B6" s="7">
         <v>200</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="0">
         <f>B6*F5</f>
         <v>600</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7">
       <c r="A7" s="5" t="s">
         <v>167</v>
       </c>
       <c r="B7" s="7">
         <v>500</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="0">
         <v>500</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" ht="30">
       <c r="A8" s="5" t="s">
         <v>168</v>
       </c>
       <c r="B8" s="6">
         <v>800</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="0">
         <f>B8*2</f>
         <v>1600</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9">
       <c r="A9" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="0">
         <v>400</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="0">
         <v>400</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10">
       <c r="A10" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="0">
         <v>600</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="0">
         <v>600</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11">
       <c r="A11" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="0">
         <v>1000</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="0">
         <v>1000</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12">
       <c r="A12" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="0">
         <v>100</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="0">
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13">
+      <c r="A13" s="0" t="s">
         <v>173</v>
       </c>
       <c r="C13" s="8">
@@ -3422,25 +3423,25 @@
         <v>12050</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14">
+      <c r="A14" s="0" t="s">
         <v>174</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="0">
         <v>12000</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="0">
         <f>C14-C13</f>
         <v>-50</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16">
       <c r="A16" s="24" t="s">
         <v>175</v>
       </c>
       <c r="B16" s="24"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17">
       <c r="A17" s="9" t="s">
         <v>162</v>
       </c>
@@ -3448,7 +3449,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18">
       <c r="A18" s="9" t="s">
         <v>164</v>
       </c>
@@ -3456,7 +3457,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" ht="30">
       <c r="A19" s="9" t="s">
         <v>166</v>
       </c>
@@ -3464,7 +3465,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20">
       <c r="A20" s="9" t="s">
         <v>167</v>
       </c>
@@ -3472,7 +3473,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" ht="30">
       <c r="A21" s="9" t="s">
         <v>179</v>
       </c>
@@ -3480,7 +3481,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22">
       <c r="A22" s="9" t="s">
         <v>169</v>
       </c>
@@ -3488,7 +3489,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23">
       <c r="A23" s="9" t="s">
         <v>170</v>
       </c>
@@ -3496,7 +3497,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24">
       <c r="A24" s="9" t="s">
         <v>171</v>
       </c>
@@ -3505,10 +3506,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells>
     <mergeCell ref="A1:E2"/>
     <mergeCell ref="A16:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added entryName and Name to the table appending. Makes appending less hardcoded
</commit_message>
<xml_diff>
--- a/FPL Luster totaloversikt.xlsx
+++ b/FPL Luster totaloversikt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\FantasyLeaguePointsFetcher\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22448540-C42C-42EB-8E56-096002AC906D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E7222A-B0F3-4D9B-B480-5199661B7C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9060" yWindow="150" windowWidth="27030" windowHeight="19815" xr2:uid="{9393CECB-8678-4F9E-A49E-EF671E63BC0A}"/>
+    <workbookView xWindow="6960" yWindow="1650" windowWidth="28800" windowHeight="15345" activeTab="2" xr2:uid="{9393CECB-8678-4F9E-A49E-EF671E63BC0A}"/>
   </bookViews>
   <sheets>
     <sheet name="GW oversikt" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="First_Day">Seiersoversikt!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029" fullCalcOnLoad="1" fullPrecision="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="184">
   <si>
     <t>Luster FPL oversikt</t>
   </si>
@@ -513,6 +513,9 @@
   </si>
   <si>
     <t>Totalutrekning</t>
+  </si>
+  <si>
+    <t>Even Høyheim  Vigdal</t>
   </si>
   <si>
     <t>Budsjett Luster FPL 24/25</t>
@@ -597,8 +600,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="16">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -813,55 +815,55 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" applyNumberFormat="0" fontId="12" applyFont="1" fillId="4" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0"/>
-    <xf numFmtId="0" applyNumberFormat="0" fontId="12" applyFont="1" fillId="5" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0"/>
-    <xf numFmtId="0" applyNumberFormat="0" fontId="13" applyFont="1" fillId="3" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0"/>
-    <xf numFmtId="0" applyNumberFormat="0" fontId="2" applyFont="1" fillId="0" applyFill="0" borderId="3" applyBorder="1" applyProtection="0" applyAlignment="0"/>
-    <xf numFmtId="0" applyNumberFormat="0" fontId="3" applyFont="1" fillId="0" applyFill="0" borderId="4" applyBorder="1" applyProtection="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyBorder="1" xfId="0"/>
-    <xf numFmtId="0" fontId="1" applyFont="1" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" applyFont="1" fillId="0" borderId="1" applyBorder="1" xfId="0"/>
-    <xf numFmtId="0" fontId="1" applyFont="1" fillId="0" borderId="2" applyBorder="1" xfId="0"/>
-    <xf numFmtId="0" fontId="5" applyFont="1" fillId="0" borderId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" applyFont="1" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" applyFont="1" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" applyFont="1" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" applyFont="1" fillId="0" borderId="0" xfId="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" applyFont="1" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" applyFont="1" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="11" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" xfId="0"/>
-    <xf numFmtId="0" fontId="11" applyFont="1" fillId="2" applyFill="1" borderId="2" applyBorder="1" xfId="0"/>
-    <xf numFmtId="0" fontId="12" applyFont="1" fillId="4" applyFill="1" borderId="5" applyBorder="1" xfId="1"/>
-    <xf numFmtId="0" fontId="0" applyFont="1" fillId="4" applyFill="1" borderId="5" applyBorder="1" xfId="1"/>
-    <xf numFmtId="0" fontId="13" applyFont="1" fillId="3" applyFill="1" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="12" applyFont="1" fillId="5" applyFill="1" borderId="5" applyBorder="1" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" applyFont="1" fillId="5" applyFill="1" borderId="5" applyBorder="1" xfId="2"/>
-    <xf numFmtId="0" fontId="0" applyFont="1" fillId="5" applyFill="1" borderId="5" applyBorder="1" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" applyFont="1" fillId="0" borderId="4" applyBorder="1" xfId="5"/>
-    <xf numFmtId="0" fontId="14" applyFont="1" fillId="0" borderId="0" applyBorder="1" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="5"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" applyFont="1" fillId="0" borderId="6" applyBorder="1" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" applyFont="1" fillId="0" borderId="3" applyBorder="1" xfId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" applyFont="1" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" applyFont="1" fillId="4" applyFill="1" borderId="5" applyBorder="1" xfId="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="20 % – uthevingsfarge 1" xfId="1" builtinId="30"/>
@@ -960,20 +962,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E90C81C4-95FC-4A01-A65E-58F76846EE81}" name="Tabell4" displayName="Tabell4" ref="A3:I28" totalsRowShown="0" headerRowDxfId="2" dataDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E90C81C4-95FC-4A01-A65E-58F76846EE81}" name="Tabell4" displayName="Tabell4" ref="A3:I28" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="A3:I28" xr:uid="{E90C81C4-95FC-4A01-A65E-58F76846EE81}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:I28">
     <sortCondition ref="B3:B28"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{9A32B1F6-F8CB-4699-B624-42469B8910F7}" name="Lagnamn" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{DF6D108C-113A-4799-B990-BC2C37720997}" name="Deltakar" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{9A32B1F6-F8CB-4699-B624-42469B8910F7}" name="Lagnamn" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{DF6D108C-113A-4799-B990-BC2C37720997}" name="Deltakar" dataDxfId="9"/>
     <tableColumn id="9" xr3:uid="{1BE17DC9-CEDA-4780-B5B9-6D2F30F3FC1E}" name="Betalt" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{C054776D-FB3B-43E4-8E3D-15A57D0CA136}" name="Rundersigera" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{B81FCAF0-57D4-419D-A6AB-2A6EF7DAF000}" name="Månadens manager" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{9D7A61DE-D7DD-449F-9053-3A41D3A70376}" name="Julecup rundesigera" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{7C2101C8-0F07-40C0-BFA8-CC10D84097B5}" name="Julecup siger" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{58C925C2-F94A-4295-B305-0F04D789387E}" name="Vinnar halvspelt" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{C054776D-FB3B-43E4-8E3D-15A57D0CA136}" name="Rundersigera" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{B81FCAF0-57D4-419D-A6AB-2A6EF7DAF000}" name="Månadens manager" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{9D7A61DE-D7DD-449F-9053-3A41D3A70376}" name="Julecup rundesigera" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{7C2101C8-0F07-40C0-BFA8-CC10D84097B5}" name="Julecup siger" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{58C925C2-F94A-4295-B305-0F04D789387E}" name="Vinnar halvspelt" dataDxfId="3"/>
     <tableColumn id="8" xr3:uid="{D494F2BF-B492-46A7-B9C3-DC48C800A910}" name="Kolonne1" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -987,7 +989,7 @@
     <sortCondition ref="B3:B27"/>
   </sortState>
   <tableColumns count="40">
-    <tableColumn id="1" xr3:uid="{74CEA007-FA61-3D40-A38E-5915AED44115}" name="Lagnamn" dataDxfId="0" dataCellStyle="Totalt"/>
+    <tableColumn id="1" xr3:uid="{74CEA007-FA61-3D40-A38E-5915AED44115}" name="Lagnamn" dataDxfId="1" dataCellStyle="Totalt"/>
     <tableColumn id="2" xr3:uid="{EB31D824-E353-F34A-AC67-139C8D0DCF1B}" name="Deltakar" dataDxfId="0" dataCellStyle="Totalt"/>
     <tableColumn id="3" xr3:uid="{07467C74-1A1C-614D-8DD7-DEF2929F0147}" name="GW1"/>
     <tableColumn id="4" xr3:uid="{905EED4D-BAD6-814F-80FA-B0DF9447BB4F}" name="GW2"/>
@@ -1351,57 +1353,57 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43A5FFB2-DF08-474B-9B68-3293440C8632}">
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="1" width="25.140625" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="23.7109375" customWidth="1"/>
-    <col min="4" max="4" bestFit="1" width="6.42578125" customWidth="1"/>
-    <col min="5" max="5" bestFit="1" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.140625" customWidth="1"/>
     <col min="7" max="7" width="16.85546875" customWidth="1"/>
-    <col min="8" max="8" bestFit="1" width="20.42578125" customWidth="1"/>
-    <col min="9" max="9" bestFit="1" width="23" customWidth="1"/>
-    <col min="10" max="11" bestFit="1" width="20.42578125" customWidth="1"/>
-    <col min="12" max="12" bestFit="1" width="23" customWidth="1"/>
-    <col min="13" max="13" bestFit="1" width="35.42578125" customWidth="1"/>
-    <col min="14" max="23" bestFit="1" width="3.7109375" customWidth="1"/>
-    <col min="24" max="24" bestFit="1" width="5.42578125" customWidth="1"/>
-    <col min="25" max="27" bestFit="1" width="3.7109375" customWidth="1"/>
-    <col min="28" max="28" bestFit="1" width="6.85546875" customWidth="1"/>
-    <col min="29" max="29" bestFit="1" width="5.42578125" customWidth="1"/>
-    <col min="30" max="30" bestFit="1" width="3.7109375" customWidth="1"/>
-    <col min="31" max="31" bestFit="1" width="6.85546875" customWidth="1"/>
-    <col min="32" max="33" bestFit="1" width="3.7109375" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="23" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="3.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15" customHeight="1">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-    </row>
-    <row r="2" ht="15" customHeight="1">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-    </row>
-    <row r="3">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+    </row>
+    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>1</v>
       </c>
@@ -1433,7 +1435,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>11</v>
       </c>
@@ -1455,7 +1457,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>16</v>
       </c>
@@ -1477,7 +1479,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>21</v>
       </c>
@@ -1489,7 +1491,7 @@
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
-      <c r="F6" s="25"/>
+      <c r="F6" s="21"/>
       <c r="G6" s="14"/>
       <c r="H6" s="14"/>
       <c r="I6" s="20" t="s">
@@ -1499,7 +1501,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="18"/>
       <c r="B7" s="18"/>
       <c r="C7" s="17"/>
@@ -1519,7 +1521,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>29</v>
       </c>
@@ -1539,7 +1541,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>33</v>
       </c>
@@ -1559,7 +1561,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>37</v>
       </c>
@@ -1579,7 +1581,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
       <c r="B11" s="18"/>
       <c r="C11" s="17"/>
@@ -1597,7 +1599,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>44</v>
       </c>
@@ -1617,7 +1619,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>48</v>
       </c>
@@ -1637,7 +1639,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>52</v>
       </c>
@@ -1657,7 +1659,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
       <c r="B15" s="18"/>
       <c r="C15" s="17"/>
@@ -1675,7 +1677,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>58</v>
       </c>
@@ -1695,7 +1697,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>61</v>
       </c>
@@ -1715,7 +1717,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>65</v>
       </c>
@@ -1735,7 +1737,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>69</v>
       </c>
@@ -1755,7 +1757,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="18"/>
       <c r="B20" s="18"/>
       <c r="C20" s="17"/>
@@ -1773,7 +1775,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="14" t="s">
         <v>76</v>
       </c>
@@ -1793,7 +1795,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
         <v>80</v>
       </c>
@@ -1813,7 +1815,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
         <v>84</v>
       </c>
@@ -1833,7 +1835,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
         <v>87</v>
       </c>
@@ -1855,7 +1857,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
         <v>92</v>
       </c>
@@ -1877,7 +1879,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="14" t="s">
         <v>96</v>
       </c>
@@ -1899,7 +1901,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="18"/>
       <c r="B27" s="18"/>
       <c r="C27" s="17"/>
@@ -1919,7 +1921,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="14" t="s">
         <v>104</v>
       </c>
@@ -1933,7 +1935,7 @@
       <c r="G28" s="14"/>
       <c r="H28" s="14"/>
     </row>
-    <row r="29">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="14" t="s">
         <v>106</v>
       </c>
@@ -1947,7 +1949,7 @@
       <c r="G29" s="14"/>
       <c r="H29" s="14"/>
     </row>
-    <row r="30">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="14" t="s">
         <v>108</v>
       </c>
@@ -1961,7 +1963,7 @@
       <c r="G30" s="14"/>
       <c r="H30" s="14"/>
     </row>
-    <row r="31">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
         <v>110</v>
       </c>
@@ -1975,7 +1977,7 @@
       <c r="G31" s="14"/>
       <c r="H31" s="14"/>
     </row>
-    <row r="32">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="18"/>
       <c r="B32" s="18"/>
       <c r="C32" s="18"/>
@@ -1987,7 +1989,7 @@
       <c r="G32" s="18"/>
       <c r="H32" s="18"/>
     </row>
-    <row r="33">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
         <v>113</v>
       </c>
@@ -2001,7 +2003,7 @@
       <c r="G33" s="14"/>
       <c r="H33" s="14"/>
     </row>
-    <row r="34">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
         <v>115</v>
       </c>
@@ -2015,7 +2017,7 @@
       <c r="G34" s="14"/>
       <c r="H34" s="14"/>
     </row>
-    <row r="35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
         <v>117</v>
       </c>
@@ -2029,7 +2031,7 @@
       <c r="G35" s="14"/>
       <c r="H35" s="14"/>
     </row>
-    <row r="36">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
         <v>119</v>
       </c>
@@ -2043,7 +2045,7 @@
       <c r="G36" s="14"/>
       <c r="H36" s="14"/>
     </row>
-    <row r="37">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="18"/>
       <c r="B37" s="18"/>
       <c r="C37" s="18"/>
@@ -2055,7 +2057,7 @@
       <c r="G37" s="18"/>
       <c r="H37" s="18"/>
     </row>
-    <row r="38">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
         <v>122</v>
       </c>
@@ -2069,7 +2071,7 @@
       <c r="G38" s="14"/>
       <c r="H38" s="14"/>
     </row>
-    <row r="39">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="14" t="s">
         <v>124</v>
       </c>
@@ -2083,7 +2085,7 @@
       <c r="G39" s="14"/>
       <c r="H39" s="14"/>
     </row>
-    <row r="40">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="18"/>
       <c r="B40" s="18"/>
       <c r="C40" s="18"/>
@@ -2095,7 +2097,7 @@
       <c r="G40" s="18"/>
       <c r="H40" s="18"/>
     </row>
-    <row r="41">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
         <v>127</v>
       </c>
@@ -2109,7 +2111,7 @@
       <c r="G41" s="14"/>
       <c r="H41" s="14"/>
     </row>
-    <row r="42">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
         <v>129</v>
       </c>
@@ -2123,7 +2125,7 @@
       <c r="G42" s="14"/>
       <c r="H42" s="14"/>
     </row>
-    <row r="43">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="14" t="s">
         <v>131</v>
       </c>
@@ -2137,7 +2139,7 @@
       <c r="G43" s="14"/>
       <c r="H43" s="14"/>
     </row>
-    <row r="44">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="14" t="s">
         <v>133</v>
       </c>
@@ -2151,7 +2153,7 @@
       <c r="G44" s="14"/>
       <c r="H44" s="14"/>
     </row>
-    <row r="45">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="14" t="s">
         <v>135</v>
       </c>
@@ -2165,7 +2167,7 @@
       <c r="G45" s="14"/>
       <c r="H45" s="14"/>
     </row>
-    <row r="46">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="18"/>
       <c r="B46" s="18"/>
       <c r="C46" s="18"/>
@@ -2177,7 +2179,7 @@
       <c r="G46" s="18"/>
       <c r="H46" s="18"/>
     </row>
-    <row r="47">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
         <v>138</v>
       </c>
@@ -2191,7 +2193,7 @@
       <c r="G47" s="14"/>
       <c r="H47" s="14"/>
     </row>
-    <row r="48">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="14" t="s">
         <v>140</v>
       </c>
@@ -2205,7 +2207,7 @@
       <c r="G48" s="14"/>
       <c r="H48" s="14"/>
     </row>
-    <row r="49">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="14" t="s">
         <v>142</v>
       </c>
@@ -2219,7 +2221,7 @@
       <c r="G49" s="14"/>
       <c r="H49" s="14"/>
     </row>
-    <row r="50">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
         <v>144</v>
       </c>
@@ -2233,7 +2235,7 @@
       <c r="G50" s="14"/>
       <c r="H50" s="14"/>
     </row>
-    <row r="51">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="18"/>
       <c r="B51" s="18"/>
       <c r="C51" s="18"/>
@@ -2246,12 +2248,11 @@
       <c r="H51" s="18"/>
     </row>
   </sheetData>
-  <mergeCells>
+  <mergeCells count="1">
     <mergeCell ref="A1:H2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
@@ -2266,41 +2267,41 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="2" max="2" bestFit="1" width="22" customWidth="1"/>
-    <col min="3" max="3" bestFit="1" width="8.42578125" customWidth="1"/>
-    <col min="4" max="4" bestFit="1" width="20.42578125" customWidth="1"/>
-    <col min="5" max="5" bestFit="1" width="19.85546875" customWidth="1"/>
-    <col min="6" max="6" bestFit="1" width="20.140625" customWidth="1"/>
-    <col min="7" max="7" bestFit="1" width="14.7109375" customWidth="1"/>
-    <col min="8" max="8" bestFit="1" width="17.7109375" customWidth="1"/>
-    <col min="9" max="9" bestFit="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
         <v>147</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-    </row>
-    <row r="3">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -2329,7 +2330,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -2346,7 +2347,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
@@ -2363,7 +2364,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
@@ -2380,7 +2381,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>27</v>
       </c>
@@ -2397,7 +2398,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>31</v>
       </c>
@@ -2414,7 +2415,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>35</v>
       </c>
@@ -2431,7 +2432,7 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>39</v>
       </c>
@@ -2448,7 +2449,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>42</v>
       </c>
@@ -2465,7 +2466,7 @@
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>46</v>
       </c>
@@ -2482,7 +2483,7 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>50</v>
       </c>
@@ -2499,7 +2500,7 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>54</v>
       </c>
@@ -2516,7 +2517,7 @@
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>56</v>
       </c>
@@ -2533,7 +2534,7 @@
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>60</v>
       </c>
@@ -2550,7 +2551,7 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>63</v>
       </c>
@@ -2567,7 +2568,7 @@
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>67</v>
       </c>
@@ -2584,7 +2585,7 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>71</v>
       </c>
@@ -2601,7 +2602,7 @@
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>74</v>
       </c>
@@ -2618,7 +2619,7 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>78</v>
       </c>
@@ -2635,7 +2636,7 @@
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>82</v>
       </c>
@@ -2652,7 +2653,7 @@
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>86</v>
       </c>
@@ -2669,7 +2670,7 @@
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>90</v>
       </c>
@@ -2686,7 +2687,7 @@
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>94</v>
       </c>
@@ -2702,7 +2703,7 @@
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>98</v>
       </c>
@@ -2718,7 +2719,7 @@
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>102</v>
       </c>
@@ -2735,7 +2736,7 @@
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -2750,12 +2751,11 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D4:D24">
     <sortCondition ref="D4:D24"/>
   </sortState>
-  <mergeCells>
+  <mergeCells count="1">
     <mergeCell ref="A1:I2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -2766,718 +2766,717 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{909B07EA-687F-744F-B9DD-893A1ABB287D}">
   <dimension ref="A1:AN27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" bestFit="1" width="21.42578125" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-    </row>
-    <row r="3">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+    </row>
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+    </row>
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G3" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="H3" t="s">
         <v>38</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="I3" t="s">
         <v>45</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="J3" t="s">
         <v>49</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="K3" t="s">
         <v>53</v>
       </c>
-      <c r="L3" s="0" t="s">
+      <c r="L3" t="s">
         <v>59</v>
       </c>
-      <c r="M3" s="0" t="s">
+      <c r="M3" t="s">
         <v>62</v>
       </c>
-      <c r="N3" s="0" t="s">
+      <c r="N3" t="s">
         <v>66</v>
       </c>
-      <c r="O3" s="0" t="s">
+      <c r="O3" t="s">
         <v>70</v>
       </c>
-      <c r="P3" s="0" t="s">
+      <c r="P3" t="s">
         <v>77</v>
       </c>
-      <c r="Q3" s="0" t="s">
+      <c r="Q3" t="s">
         <v>81</v>
       </c>
-      <c r="R3" s="0" t="s">
+      <c r="R3" t="s">
         <v>85</v>
       </c>
-      <c r="S3" s="0" t="s">
+      <c r="S3" t="s">
         <v>88</v>
       </c>
-      <c r="T3" s="0" t="s">
+      <c r="T3" t="s">
         <v>93</v>
       </c>
-      <c r="U3" s="0" t="s">
+      <c r="U3" t="s">
         <v>97</v>
       </c>
-      <c r="V3" s="0" t="s">
+      <c r="V3" t="s">
         <v>105</v>
       </c>
-      <c r="W3" s="0" t="s">
+      <c r="W3" t="s">
         <v>107</v>
       </c>
-      <c r="X3" s="0" t="s">
+      <c r="X3" t="s">
         <v>109</v>
       </c>
-      <c r="Y3" s="0" t="s">
+      <c r="Y3" t="s">
         <v>111</v>
       </c>
-      <c r="Z3" s="0" t="s">
+      <c r="Z3" t="s">
         <v>114</v>
       </c>
-      <c r="AA3" s="0" t="s">
+      <c r="AA3" t="s">
         <v>116</v>
       </c>
-      <c r="AB3" s="0" t="s">
+      <c r="AB3" t="s">
         <v>118</v>
       </c>
-      <c r="AC3" s="0" t="s">
+      <c r="AC3" t="s">
         <v>120</v>
       </c>
-      <c r="AD3" s="0" t="s">
+      <c r="AD3" t="s">
         <v>123</v>
       </c>
-      <c r="AE3" s="0" t="s">
+      <c r="AE3" t="s">
         <v>125</v>
       </c>
-      <c r="AF3" s="0" t="s">
+      <c r="AF3" t="s">
         <v>128</v>
       </c>
-      <c r="AG3" s="0" t="s">
+      <c r="AG3" t="s">
         <v>130</v>
       </c>
-      <c r="AH3" s="0" t="s">
+      <c r="AH3" t="s">
         <v>132</v>
       </c>
-      <c r="AI3" s="0" t="s">
+      <c r="AI3" t="s">
         <v>134</v>
       </c>
-      <c r="AJ3" s="0" t="s">
+      <c r="AJ3" t="s">
         <v>136</v>
       </c>
-      <c r="AK3" s="0" t="s">
+      <c r="AK3" t="s">
         <v>139</v>
       </c>
-      <c r="AL3" s="0" t="s">
+      <c r="AL3" t="s">
         <v>141</v>
       </c>
-      <c r="AM3" s="0" t="s">
+      <c r="AM3" t="s">
         <v>143</v>
       </c>
-      <c r="AN3" s="0" t="s">
+      <c r="AN3" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="0" t="s">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="0">
+      <c r="C4">
         <v>67</v>
       </c>
-      <c r="D4" s="0">
+      <c r="D4">
         <v>66</v>
       </c>
-      <c r="E4" s="0">
+      <c r="E4">
         <v>85</v>
       </c>
-      <c r="F4" s="0">
+      <c r="F4">
         <v>49</v>
       </c>
-      <c r="G4" s="0">
+      <c r="G4">
         <v>66</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="0" t="s">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="0">
+      <c r="C5">
         <v>61</v>
       </c>
-      <c r="D5" s="0">
+      <c r="D5">
         <v>75</v>
       </c>
-      <c r="E5" s="0">
+      <c r="E5">
         <v>68</v>
       </c>
-      <c r="F5" s="0">
+      <c r="F5">
         <v>63</v>
       </c>
-      <c r="G5" s="0">
+      <c r="G5">
         <v>88</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="0" t="s">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="0">
+      <c r="C6">
         <v>69</v>
       </c>
-      <c r="D6" s="0">
+      <c r="D6">
         <v>76</v>
       </c>
-      <c r="E6" s="0">
+      <c r="E6">
         <v>76</v>
       </c>
-      <c r="F6" s="0">
+      <c r="F6">
         <v>51</v>
       </c>
-      <c r="G6" s="0">
+      <c r="G6">
         <v>82</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="0" t="s">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="0">
+      <c r="C7">
         <v>70</v>
       </c>
-      <c r="D7" s="0">
+      <c r="D7">
         <v>78</v>
       </c>
-      <c r="E7" s="0">
+      <c r="E7">
         <v>74</v>
       </c>
-      <c r="F7" s="0">
+      <c r="F7">
         <v>60</v>
       </c>
-      <c r="G7" s="0">
+      <c r="G7">
         <v>58</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="0" t="s">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="0">
+      <c r="C8">
         <v>75</v>
       </c>
-      <c r="D8" s="0">
+      <c r="D8">
         <v>69</v>
       </c>
-      <c r="E8" s="0">
+      <c r="E8">
         <v>73</v>
       </c>
-      <c r="F8" s="0">
+      <c r="F8">
         <v>33</v>
       </c>
-      <c r="G8" s="0">
+      <c r="G8">
         <v>39</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="0" t="s">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="0">
+      <c r="B9" t="s">
+        <v>157</v>
+      </c>
+      <c r="C9">
         <v>45</v>
       </c>
-      <c r="D9" s="0">
+      <c r="D9">
         <v>73</v>
       </c>
-      <c r="E9" s="0">
+      <c r="E9">
         <v>78</v>
       </c>
-      <c r="F9" s="0">
+      <c r="F9">
         <v>50</v>
       </c>
-      <c r="G9" s="0">
+      <c r="G9">
         <v>62</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="0" t="s">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="0">
+      <c r="C10">
         <v>64</v>
       </c>
-      <c r="D10" s="0">
+      <c r="D10">
         <v>41</v>
       </c>
-      <c r="E10" s="0">
+      <c r="E10">
         <v>40</v>
       </c>
-      <c r="F10" s="0">
+      <c r="F10">
         <v>50</v>
       </c>
-      <c r="G10" s="0">
+      <c r="G10">
         <v>54</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="0" t="s">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="0">
+      <c r="C11">
         <v>67</v>
       </c>
-      <c r="D11" s="0">
+      <c r="D11">
         <v>71</v>
       </c>
-      <c r="E11" s="0">
+      <c r="E11">
         <v>64</v>
       </c>
-      <c r="F11" s="0">
+      <c r="F11">
         <v>52</v>
       </c>
-      <c r="G11" s="0">
+      <c r="G11">
         <v>65</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" s="0" t="s">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="0">
+      <c r="C12">
         <v>48</v>
       </c>
-      <c r="D12" s="0">
+      <c r="D12">
         <v>76</v>
       </c>
-      <c r="E12" s="0">
+      <c r="E12">
         <v>62</v>
       </c>
-      <c r="F12" s="0">
+      <c r="F12">
         <v>86</v>
       </c>
-      <c r="G12" s="0">
+      <c r="G12">
         <v>45</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="0" t="s">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="0">
+      <c r="C13">
         <v>57</v>
       </c>
-      <c r="D13" s="0">
+      <c r="D13">
         <v>62</v>
       </c>
-      <c r="E13" s="0">
+      <c r="E13">
         <v>71</v>
       </c>
-      <c r="F13" s="0">
+      <c r="F13">
         <v>48</v>
       </c>
-      <c r="G13" s="0">
+      <c r="G13">
         <v>61</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="0" t="s">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>54</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="0">
+      <c r="C14">
         <v>84</v>
       </c>
-      <c r="D14" s="0">
+      <c r="D14">
         <v>53</v>
       </c>
-      <c r="E14" s="0">
+      <c r="E14">
         <v>85</v>
       </c>
-      <c r="F14" s="0">
+      <c r="F14">
         <v>37</v>
       </c>
-      <c r="G14" s="0">
+      <c r="G14">
         <v>69</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="0" t="s">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>56</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="0">
+      <c r="C15">
         <v>55</v>
       </c>
-      <c r="D15" s="0">
+      <c r="D15">
         <v>33</v>
       </c>
-      <c r="E15" s="0">
+      <c r="E15">
         <v>69</v>
       </c>
-      <c r="F15" s="0">
+      <c r="F15">
         <v>65</v>
       </c>
-      <c r="G15" s="0">
+      <c r="G15">
         <v>66</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="0" t="s">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="0">
+      <c r="C16">
         <v>75</v>
       </c>
-      <c r="D16" s="0">
+      <c r="D16">
         <v>98</v>
       </c>
-      <c r="E16" s="0">
+      <c r="E16">
         <v>69</v>
       </c>
-      <c r="F16" s="0">
+      <c r="F16">
         <v>59</v>
       </c>
-      <c r="G16" s="0">
+      <c r="G16">
         <v>56</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="0" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>63</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="0">
+      <c r="C17">
         <v>79</v>
       </c>
-      <c r="D17" s="0">
+      <c r="D17">
         <v>79</v>
       </c>
-      <c r="E17" s="0">
+      <c r="E17">
         <v>73</v>
       </c>
-      <c r="F17" s="0">
+      <c r="F17">
         <v>60</v>
       </c>
-      <c r="G17" s="0">
+      <c r="G17">
         <v>83</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="0" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>67</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" t="s">
         <v>68</v>
       </c>
-      <c r="C18" s="0">
+      <c r="C18">
         <v>53</v>
       </c>
-      <c r="D18" s="0">
+      <c r="D18">
         <v>73</v>
       </c>
-      <c r="E18" s="0">
+      <c r="E18">
         <v>75</v>
       </c>
-      <c r="F18" s="0">
+      <c r="F18">
         <v>40</v>
       </c>
-      <c r="G18" s="0">
+      <c r="G18">
         <v>51</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" s="0" t="s">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>71</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" t="s">
         <v>72</v>
       </c>
-      <c r="C19" s="0">
+      <c r="C19">
         <v>68</v>
       </c>
-      <c r="D19" s="0">
+      <c r="D19">
         <v>82</v>
       </c>
-      <c r="E19" s="0">
+      <c r="E19">
         <v>66</v>
       </c>
-      <c r="F19" s="0">
+      <c r="F19">
         <v>53</v>
       </c>
-      <c r="G19" s="0">
+      <c r="G19">
         <v>77</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="0" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>74</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" t="s">
         <v>75</v>
       </c>
-      <c r="C20" s="0">
+      <c r="C20">
         <v>76</v>
       </c>
-      <c r="D20" s="0">
+      <c r="D20">
         <v>74</v>
       </c>
-      <c r="E20" s="0">
+      <c r="E20">
         <v>69</v>
       </c>
-      <c r="F20" s="0">
+      <c r="F20">
         <v>56</v>
       </c>
-      <c r="G20" s="0">
+      <c r="G20">
         <v>62</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" s="0" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>78</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" t="s">
         <v>79</v>
       </c>
-      <c r="C21" s="0">
+      <c r="C21">
         <v>42</v>
       </c>
-      <c r="D21" s="0">
+      <c r="D21">
         <v>68</v>
       </c>
-      <c r="E21" s="0">
+      <c r="E21">
         <v>68</v>
       </c>
-      <c r="F21" s="0">
+      <c r="F21">
         <v>61</v>
       </c>
-      <c r="G21" s="0">
+      <c r="G21">
         <v>50</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" s="0" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>102</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" t="s">
         <v>103</v>
       </c>
-      <c r="C22" s="0">
+      <c r="C22">
         <v>60</v>
       </c>
-      <c r="D22" s="0">
+      <c r="D22">
         <v>81</v>
       </c>
-      <c r="E22" s="0">
+      <c r="E22">
         <v>71</v>
       </c>
-      <c r="F22" s="0">
+      <c r="F22">
         <v>45</v>
       </c>
-      <c r="G22" s="0">
+      <c r="G22">
         <v>67</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" s="0" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>82</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" t="s">
         <v>83</v>
       </c>
-      <c r="C23" s="0">
+      <c r="C23">
         <v>81</v>
       </c>
-      <c r="D23" s="0">
+      <c r="D23">
         <v>71</v>
       </c>
-      <c r="E23" s="0">
+      <c r="E23">
         <v>85</v>
       </c>
-      <c r="F23" s="0">
+      <c r="F23">
         <v>48</v>
       </c>
-      <c r="G23" s="0">
+      <c r="G23">
         <v>61</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="0" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>86</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="0">
+      <c r="C24">
         <v>72</v>
       </c>
-      <c r="D24" s="0">
+      <c r="D24">
         <v>77</v>
       </c>
-      <c r="E24" s="0">
+      <c r="E24">
         <v>95</v>
       </c>
-      <c r="F24" s="0">
+      <c r="F24">
         <v>40</v>
       </c>
-      <c r="G24" s="0">
+      <c r="G24">
         <v>61</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" s="0" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>90</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" t="s">
         <v>91</v>
       </c>
-      <c r="C25" s="0">
+      <c r="C25">
         <v>62</v>
       </c>
-      <c r="D25" s="0">
+      <c r="D25">
         <v>45</v>
       </c>
-      <c r="E25" s="0">
+      <c r="E25">
         <v>38</v>
       </c>
-      <c r="F25" s="0">
+      <c r="F25">
         <v>38</v>
       </c>
-      <c r="G25" s="0">
+      <c r="G25">
         <v>35</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" s="0" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>94</v>
       </c>
-      <c r="B26" s="0" t="s">
+      <c r="B26" t="s">
         <v>95</v>
       </c>
-      <c r="C26" s="0">
+      <c r="C26">
         <v>54</v>
       </c>
-      <c r="D26" s="0">
+      <c r="D26">
         <v>78</v>
       </c>
-      <c r="E26" s="0">
+      <c r="E26">
         <v>84</v>
       </c>
-      <c r="F26" s="0">
+      <c r="F26">
         <v>56</v>
       </c>
-      <c r="G26" s="0">
+      <c r="G26">
         <v>63</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" s="0" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>98</v>
       </c>
-      <c r="B27" s="0" t="s">
+      <c r="B27" t="s">
         <v>99</v>
       </c>
-      <c r="C27" s="0">
+      <c r="C27">
         <v>48</v>
       </c>
-      <c r="D27" s="0">
+      <c r="D27">
         <v>90</v>
       </c>
-      <c r="E27" s="0">
+      <c r="E27">
         <v>89</v>
       </c>
-      <c r="F27" s="0">
+      <c r="F27">
         <v>53</v>
       </c>
-      <c r="G27" s="0">
+      <c r="G27">
         <v>75</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells>
+  <mergeCells count="1">
     <mergeCell ref="A1:G2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0"/>
-  <headerFooter/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -3495,254 +3494,253 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.140625" customWidth="1"/>
-    <col min="5" max="5" bestFit="1" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="23" t="s">
-        <v>157</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="0" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
         <v>158</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>159</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="B3" t="s">
         <v>160</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="C3" t="s">
         <v>161</v>
       </c>
-      <c r="F3" s="0">
+      <c r="E3" t="s">
+        <v>162</v>
+      </c>
+      <c r="F3">
         <v>38</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B4" s="7">
         <v>125</v>
       </c>
-      <c r="C4" s="0">
+      <c r="C4">
         <f>B4*F3</f>
         <v>4750</v>
       </c>
-      <c r="E4" s="0" t="s">
-        <v>163</v>
-      </c>
-      <c r="F4" s="0">
+      <c r="E4" t="s">
+        <v>164</v>
+      </c>
+      <c r="F4">
         <v>10</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B5" s="7">
         <v>250</v>
       </c>
-      <c r="C5" s="0">
+      <c r="C5">
         <f>B5*F4</f>
         <v>2500</v>
       </c>
-      <c r="E5" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="F5" s="0">
+      <c r="E5" t="s">
+        <v>166</v>
+      </c>
+      <c r="F5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" ht="30">
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B6" s="7">
         <v>200</v>
       </c>
-      <c r="C6" s="0">
+      <c r="C6">
         <f>B6*F5</f>
         <v>600</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B7" s="7">
         <v>500</v>
       </c>
-      <c r="C7" s="0">
+      <c r="C7">
         <v>500</v>
       </c>
     </row>
-    <row r="8" ht="30">
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B8" s="6">
         <v>800</v>
       </c>
-      <c r="C8" s="0">
+      <c r="C8">
         <f>B8*2</f>
         <v>1600</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="B9" s="0">
+        <v>170</v>
+      </c>
+      <c r="B9">
         <v>400</v>
       </c>
-      <c r="C9" s="0">
+      <c r="C9">
         <v>400</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="B10" s="0">
+        <v>171</v>
+      </c>
+      <c r="B10">
         <v>600</v>
       </c>
-      <c r="C10" s="0">
+      <c r="C10">
         <v>600</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="B11" s="0">
+        <v>172</v>
+      </c>
+      <c r="B11">
         <v>1000</v>
       </c>
-      <c r="C11" s="0">
+      <c r="C11">
         <v>1000</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="B12" s="0">
+        <v>173</v>
+      </c>
+      <c r="B12">
         <v>100</v>
       </c>
-      <c r="C12" s="0">
+      <c r="C12">
         <v>100</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="0" t="s">
-        <v>173</v>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>174</v>
       </c>
       <c r="C13" s="8">
         <f>SUM(C4:C12)</f>
         <v>12050</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="0" t="s">
-        <v>174</v>
-      </c>
-      <c r="C14" s="0">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>175</v>
+      </c>
+      <c r="C14">
         <v>12000</v>
       </c>
-      <c r="D14" s="0">
+      <c r="D14">
         <f>C14-C13</f>
         <v>-50</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="24" t="s">
-        <v>175</v>
-      </c>
-      <c r="B16" s="24"/>
-    </row>
-    <row r="17">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="25" t="s">
+        <v>176</v>
+      </c>
+      <c r="B16" s="25"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="19" ht="30">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="21" ht="30">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="B22" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="B21" s="11" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="23">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="24">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells>
+  <mergeCells count="2">
     <mergeCell ref="A1:E2"/>
     <mergeCell ref="A16:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
reformatted code to make it more best practice and moar readability
</commit_message>
<xml_diff>
--- a/FPL Luster totaloversikt.xlsx
+++ b/FPL Luster totaloversikt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\FantasyLeaguePointsFetcher\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E7222A-B0F3-4D9B-B480-5199661B7C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A550ED9C-6AE0-429B-A793-1D215819B771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6960" yWindow="1650" windowWidth="28800" windowHeight="15345" activeTab="2" xr2:uid="{9393CECB-8678-4F9E-A49E-EF671E63BC0A}"/>
   </bookViews>
@@ -21,7 +21,7 @@
   <definedNames>
     <definedName name="First_Day">Seiersoversikt!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1" fullPrecision="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="184">
   <si>
     <t>Luster FPL oversikt</t>
   </si>
@@ -515,7 +515,7 @@
     <t>Totalutrekning</t>
   </si>
   <si>
-    <t>Even Høyheim  Vigdal</t>
+    <t xml:space="preserve">Even Høyheim  Vigdal</t>
   </si>
   <si>
     <t>Budsjett Luster FPL 24/25</t>
@@ -600,7 +600,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -815,53 +816,53 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="12" applyFont="1" fillId="4" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0"/>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="12" applyFont="1" fillId="5" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0"/>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="13" applyFont="1" fillId="3" applyFill="1" borderId="0" applyBorder="0" applyProtection="0" applyAlignment="0"/>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="2" applyFont="1" fillId="0" applyFill="0" borderId="3" applyBorder="1" applyProtection="0" applyAlignment="0"/>
+    <xf numFmtId="0" applyNumberFormat="0" fontId="3" applyFont="1" fillId="0" applyFill="0" borderId="4" applyBorder="1" applyProtection="0" applyAlignment="0"/>
   </cellStyleXfs>
   <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" fontId="1" applyFont="1" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" applyFont="1" fillId="0" borderId="1" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" fontId="1" applyFont="1" fillId="0" borderId="2" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" fontId="5" applyFont="1" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" applyFont="1" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" applyFont="1" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" applyFont="1" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="9" applyFont="1" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" applyFont="1" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="10" applyFont="1" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="11" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" fontId="11" applyFont="1" fillId="2" applyFill="1" borderId="2" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" fontId="12" applyFont="1" fillId="4" applyFill="1" borderId="5" applyBorder="1" xfId="1"/>
+    <xf numFmtId="0" fontId="0" applyFont="1" fillId="4" applyFill="1" borderId="5" applyBorder="1" xfId="1"/>
+    <xf numFmtId="0" fontId="13" applyFont="1" fillId="3" applyFill="1" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="12" applyFont="1" fillId="5" applyFill="1" borderId="5" applyBorder="1" xfId="2" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" applyFont="1" fillId="5" applyFill="1" borderId="5" applyBorder="1" xfId="2"/>
+    <xf numFmtId="0" fontId="0" applyFont="1" fillId="5" applyFill="1" borderId="5" applyBorder="1" xfId="2" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="5"/>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" applyFont="1" fillId="0" borderId="4" applyBorder="1" xfId="5"/>
+    <xf numFmtId="0" fontId="15" applyFont="1" fillId="4" applyFill="1" borderId="5" applyBorder="1" xfId="1"/>
+    <xf numFmtId="0" fontId="14" applyFont="1" fillId="0" borderId="0" applyBorder="1" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" applyFont="1" fillId="0" borderId="6" applyBorder="1" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="4" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" applyFont="1" fillId="0" borderId="3" applyBorder="1" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" applyFont="1" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -962,20 +963,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E90C81C4-95FC-4A01-A65E-58F76846EE81}" name="Tabell4" displayName="Tabell4" ref="A3:I28" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E90C81C4-95FC-4A01-A65E-58F76846EE81}" name="Tabell4" displayName="Tabell4" ref="A3:I28" totalsRowShown="0" headerRowDxfId="2" dataDxfId="2">
   <autoFilter ref="A3:I28" xr:uid="{E90C81C4-95FC-4A01-A65E-58F76846EE81}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:I28">
     <sortCondition ref="B3:B28"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{9A32B1F6-F8CB-4699-B624-42469B8910F7}" name="Lagnamn" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{DF6D108C-113A-4799-B990-BC2C37720997}" name="Deltakar" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{9A32B1F6-F8CB-4699-B624-42469B8910F7}" name="Lagnamn" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{DF6D108C-113A-4799-B990-BC2C37720997}" name="Deltakar" dataDxfId="2"/>
     <tableColumn id="9" xr3:uid="{1BE17DC9-CEDA-4780-B5B9-6D2F30F3FC1E}" name="Betalt" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{C054776D-FB3B-43E4-8E3D-15A57D0CA136}" name="Rundersigera" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{B81FCAF0-57D4-419D-A6AB-2A6EF7DAF000}" name="Månadens manager" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{9D7A61DE-D7DD-449F-9053-3A41D3A70376}" name="Julecup rundesigera" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{7C2101C8-0F07-40C0-BFA8-CC10D84097B5}" name="Julecup siger" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{58C925C2-F94A-4295-B305-0F04D789387E}" name="Vinnar halvspelt" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{C054776D-FB3B-43E4-8E3D-15A57D0CA136}" name="Rundersigera" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{B81FCAF0-57D4-419D-A6AB-2A6EF7DAF000}" name="Månadens manager" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{9D7A61DE-D7DD-449F-9053-3A41D3A70376}" name="Julecup rundesigera" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{7C2101C8-0F07-40C0-BFA8-CC10D84097B5}" name="Julecup siger" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{58C925C2-F94A-4295-B305-0F04D789387E}" name="Vinnar halvspelt" dataDxfId="2"/>
     <tableColumn id="8" xr3:uid="{D494F2BF-B492-46A7-B9C3-DC48C800A910}" name="Kolonne1" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -989,7 +990,7 @@
     <sortCondition ref="B3:B27"/>
   </sortState>
   <tableColumns count="40">
-    <tableColumn id="1" xr3:uid="{74CEA007-FA61-3D40-A38E-5915AED44115}" name="Lagnamn" dataDxfId="1" dataCellStyle="Totalt"/>
+    <tableColumn id="1" xr3:uid="{74CEA007-FA61-3D40-A38E-5915AED44115}" name="Lagnamn" dataDxfId="0" dataCellStyle="Totalt"/>
     <tableColumn id="2" xr3:uid="{EB31D824-E353-F34A-AC67-139C8D0DCF1B}" name="Deltakar" dataDxfId="0" dataCellStyle="Totalt"/>
     <tableColumn id="3" xr3:uid="{07467C74-1A1C-614D-8DD7-DEF2929F0147}" name="GW1"/>
     <tableColumn id="4" xr3:uid="{905EED4D-BAD6-814F-80FA-B0DF9447BB4F}" name="GW2"/>
@@ -1359,29 +1360,29 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="1" width="25.140625" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="23.7109375" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" bestFit="1" width="6.42578125" customWidth="1"/>
+    <col min="5" max="5" bestFit="1" width="18.42578125" customWidth="1"/>
     <col min="6" max="6" width="19.140625" customWidth="1"/>
     <col min="7" max="7" width="16.85546875" customWidth="1"/>
-    <col min="8" max="8" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="23" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="27" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" bestFit="1" width="20.42578125" customWidth="1"/>
+    <col min="9" max="9" bestFit="1" width="23" customWidth="1"/>
+    <col min="10" max="11" bestFit="1" width="20.42578125" customWidth="1"/>
+    <col min="12" max="12" bestFit="1" width="23" customWidth="1"/>
+    <col min="13" max="13" bestFit="1" width="35.42578125" customWidth="1"/>
+    <col min="14" max="23" bestFit="1" width="3.7109375" customWidth="1"/>
+    <col min="24" max="24" bestFit="1" width="5.42578125" customWidth="1"/>
+    <col min="25" max="27" bestFit="1" width="3.7109375" customWidth="1"/>
+    <col min="28" max="28" bestFit="1" width="6.85546875" customWidth="1"/>
+    <col min="29" max="29" bestFit="1" width="5.42578125" customWidth="1"/>
+    <col min="30" max="30" bestFit="1" width="3.7109375" customWidth="1"/>
+    <col min="31" max="31" bestFit="1" width="6.85546875" customWidth="1"/>
+    <col min="32" max="33" bestFit="1" width="3.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" ht="15" customHeight="1">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
@@ -1393,7 +1394,7 @@
       <c r="G1" s="22"/>
       <c r="H1" s="22"/>
     </row>
-    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" ht="15" customHeight="1">
       <c r="A2" s="23"/>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
@@ -1403,7 +1404,7 @@
       <c r="G2" s="23"/>
       <c r="H2" s="23"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3">
       <c r="A3" s="14" t="s">
         <v>1</v>
       </c>
@@ -1435,7 +1436,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4">
       <c r="A4" s="14" t="s">
         <v>11</v>
       </c>
@@ -1457,7 +1458,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5">
       <c r="A5" s="14" t="s">
         <v>16</v>
       </c>
@@ -1479,7 +1480,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6">
       <c r="A6" s="14" t="s">
         <v>21</v>
       </c>
@@ -1501,7 +1502,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7">
       <c r="A7" s="18"/>
       <c r="B7" s="18"/>
       <c r="C7" s="17"/>
@@ -1521,7 +1522,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8">
       <c r="A8" s="14" t="s">
         <v>29</v>
       </c>
@@ -1541,7 +1542,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9">
       <c r="A9" s="14" t="s">
         <v>33</v>
       </c>
@@ -1561,7 +1562,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10">
       <c r="A10" s="14" t="s">
         <v>37</v>
       </c>
@@ -1581,7 +1582,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11">
       <c r="A11" s="18"/>
       <c r="B11" s="18"/>
       <c r="C11" s="17"/>
@@ -1599,7 +1600,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12">
       <c r="A12" s="14" t="s">
         <v>44</v>
       </c>
@@ -1619,7 +1620,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13">
       <c r="A13" s="14" t="s">
         <v>48</v>
       </c>
@@ -1639,7 +1640,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14">
       <c r="A14" s="14" t="s">
         <v>52</v>
       </c>
@@ -1659,7 +1660,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15">
       <c r="A15" s="18"/>
       <c r="B15" s="18"/>
       <c r="C15" s="17"/>
@@ -1677,7 +1678,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16">
       <c r="A16" s="14" t="s">
         <v>58</v>
       </c>
@@ -1697,7 +1698,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17">
       <c r="A17" s="14" t="s">
         <v>61</v>
       </c>
@@ -1717,7 +1718,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18">
       <c r="A18" s="14" t="s">
         <v>65</v>
       </c>
@@ -1737,7 +1738,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19">
       <c r="A19" s="14" t="s">
         <v>69</v>
       </c>
@@ -1757,7 +1758,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20">
       <c r="A20" s="18"/>
       <c r="B20" s="18"/>
       <c r="C20" s="17"/>
@@ -1775,7 +1776,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21">
       <c r="A21" s="14" t="s">
         <v>76</v>
       </c>
@@ -1795,7 +1796,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22">
       <c r="A22" s="14" t="s">
         <v>80</v>
       </c>
@@ -1815,7 +1816,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23">
       <c r="A23" s="14" t="s">
         <v>84</v>
       </c>
@@ -1835,7 +1836,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24">
       <c r="A24" s="14" t="s">
         <v>87</v>
       </c>
@@ -1857,7 +1858,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25">
       <c r="A25" s="14" t="s">
         <v>92</v>
       </c>
@@ -1879,7 +1880,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26">
       <c r="A26" s="14" t="s">
         <v>96</v>
       </c>
@@ -1901,7 +1902,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27">
       <c r="A27" s="18"/>
       <c r="B27" s="18"/>
       <c r="C27" s="17"/>
@@ -1921,7 +1922,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28">
       <c r="A28" s="14" t="s">
         <v>104</v>
       </c>
@@ -1935,7 +1936,7 @@
       <c r="G28" s="14"/>
       <c r="H28" s="14"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29">
       <c r="A29" s="14" t="s">
         <v>106</v>
       </c>
@@ -1949,7 +1950,7 @@
       <c r="G29" s="14"/>
       <c r="H29" s="14"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30">
       <c r="A30" s="14" t="s">
         <v>108</v>
       </c>
@@ -1963,7 +1964,7 @@
       <c r="G30" s="14"/>
       <c r="H30" s="14"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31">
       <c r="A31" s="14" t="s">
         <v>110</v>
       </c>
@@ -1977,7 +1978,7 @@
       <c r="G31" s="14"/>
       <c r="H31" s="14"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32">
       <c r="A32" s="18"/>
       <c r="B32" s="18"/>
       <c r="C32" s="18"/>
@@ -1989,7 +1990,7 @@
       <c r="G32" s="18"/>
       <c r="H32" s="18"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33">
       <c r="A33" s="14" t="s">
         <v>113</v>
       </c>
@@ -2003,7 +2004,7 @@
       <c r="G33" s="14"/>
       <c r="H33" s="14"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34">
       <c r="A34" s="14" t="s">
         <v>115</v>
       </c>
@@ -2017,7 +2018,7 @@
       <c r="G34" s="14"/>
       <c r="H34" s="14"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35">
       <c r="A35" s="14" t="s">
         <v>117</v>
       </c>
@@ -2031,7 +2032,7 @@
       <c r="G35" s="14"/>
       <c r="H35" s="14"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36">
       <c r="A36" s="14" t="s">
         <v>119</v>
       </c>
@@ -2045,7 +2046,7 @@
       <c r="G36" s="14"/>
       <c r="H36" s="14"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37">
       <c r="A37" s="18"/>
       <c r="B37" s="18"/>
       <c r="C37" s="18"/>
@@ -2057,7 +2058,7 @@
       <c r="G37" s="18"/>
       <c r="H37" s="18"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38">
       <c r="A38" s="14" t="s">
         <v>122</v>
       </c>
@@ -2071,7 +2072,7 @@
       <c r="G38" s="14"/>
       <c r="H38" s="14"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39">
       <c r="A39" s="14" t="s">
         <v>124</v>
       </c>
@@ -2085,7 +2086,7 @@
       <c r="G39" s="14"/>
       <c r="H39" s="14"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40">
       <c r="A40" s="18"/>
       <c r="B40" s="18"/>
       <c r="C40" s="18"/>
@@ -2097,7 +2098,7 @@
       <c r="G40" s="18"/>
       <c r="H40" s="18"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41">
       <c r="A41" s="14" t="s">
         <v>127</v>
       </c>
@@ -2111,7 +2112,7 @@
       <c r="G41" s="14"/>
       <c r="H41" s="14"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42">
       <c r="A42" s="14" t="s">
         <v>129</v>
       </c>
@@ -2125,7 +2126,7 @@
       <c r="G42" s="14"/>
       <c r="H42" s="14"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43">
       <c r="A43" s="14" t="s">
         <v>131</v>
       </c>
@@ -2139,7 +2140,7 @@
       <c r="G43" s="14"/>
       <c r="H43" s="14"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44">
       <c r="A44" s="14" t="s">
         <v>133</v>
       </c>
@@ -2153,7 +2154,7 @@
       <c r="G44" s="14"/>
       <c r="H44" s="14"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45">
       <c r="A45" s="14" t="s">
         <v>135</v>
       </c>
@@ -2167,7 +2168,7 @@
       <c r="G45" s="14"/>
       <c r="H45" s="14"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46">
       <c r="A46" s="18"/>
       <c r="B46" s="18"/>
       <c r="C46" s="18"/>
@@ -2179,7 +2180,7 @@
       <c r="G46" s="18"/>
       <c r="H46" s="18"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47">
       <c r="A47" s="14" t="s">
         <v>138</v>
       </c>
@@ -2193,7 +2194,7 @@
       <c r="G47" s="14"/>
       <c r="H47" s="14"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48">
       <c r="A48" s="14" t="s">
         <v>140</v>
       </c>
@@ -2207,7 +2208,7 @@
       <c r="G48" s="14"/>
       <c r="H48" s="14"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49">
       <c r="A49" s="14" t="s">
         <v>142</v>
       </c>
@@ -2221,7 +2222,7 @@
       <c r="G49" s="14"/>
       <c r="H49" s="14"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50">
       <c r="A50" s="14" t="s">
         <v>144</v>
       </c>
@@ -2235,7 +2236,7 @@
       <c r="G50" s="14"/>
       <c r="H50" s="14"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51">
       <c r="A51" s="18"/>
       <c r="B51" s="18"/>
       <c r="C51" s="18"/>
@@ -2248,11 +2249,12 @@
       <c r="H51" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells>
     <mergeCell ref="A1:H2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
@@ -2267,17 +2269,17 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="1" width="22" customWidth="1"/>
+    <col min="3" max="3" bestFit="1" width="8.42578125" customWidth="1"/>
+    <col min="4" max="4" bestFit="1" width="20.42578125" customWidth="1"/>
+    <col min="5" max="5" bestFit="1" width="19.85546875" customWidth="1"/>
+    <col min="6" max="6" bestFit="1" width="20.140625" customWidth="1"/>
+    <col min="7" max="7" bestFit="1" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" bestFit="1" width="17.7109375" customWidth="1"/>
+    <col min="9" max="9" bestFit="1" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" s="24" t="s">
         <v>147</v>
       </c>
@@ -2290,7 +2292,7 @@
       <c r="H1" s="24"/>
       <c r="I1" s="24"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2">
       <c r="A2" s="24"/>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
@@ -2301,7 +2303,7 @@
       <c r="H2" s="24"/>
       <c r="I2" s="24"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -2330,7 +2332,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -2347,7 +2349,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5">
       <c r="A5" s="2" t="s">
         <v>19</v>
       </c>
@@ -2364,7 +2366,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6">
       <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
@@ -2381,7 +2383,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7">
       <c r="A7" s="2" t="s">
         <v>27</v>
       </c>
@@ -2398,7 +2400,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8">
       <c r="A8" s="2" t="s">
         <v>31</v>
       </c>
@@ -2415,7 +2417,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9">
       <c r="A9" s="2" t="s">
         <v>35</v>
       </c>
@@ -2432,7 +2434,7 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10">
       <c r="A10" s="2" t="s">
         <v>39</v>
       </c>
@@ -2449,7 +2451,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11">
       <c r="A11" s="2" t="s">
         <v>42</v>
       </c>
@@ -2466,7 +2468,7 @@
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12">
       <c r="A12" s="2" t="s">
         <v>46</v>
       </c>
@@ -2483,7 +2485,7 @@
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13">
       <c r="A13" s="2" t="s">
         <v>50</v>
       </c>
@@ -2500,7 +2502,7 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14">
       <c r="A14" s="2" t="s">
         <v>54</v>
       </c>
@@ -2517,7 +2519,7 @@
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15">
       <c r="A15" s="2" t="s">
         <v>56</v>
       </c>
@@ -2534,7 +2536,7 @@
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16">
       <c r="A16" s="2" t="s">
         <v>60</v>
       </c>
@@ -2551,7 +2553,7 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17">
       <c r="A17" s="2" t="s">
         <v>63</v>
       </c>
@@ -2568,7 +2570,7 @@
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18">
       <c r="A18" s="2" t="s">
         <v>67</v>
       </c>
@@ -2585,7 +2587,7 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19">
       <c r="A19" s="2" t="s">
         <v>71</v>
       </c>
@@ -2602,7 +2604,7 @@
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20">
       <c r="A20" s="2" t="s">
         <v>74</v>
       </c>
@@ -2619,7 +2621,7 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21">
       <c r="A21" s="2" t="s">
         <v>78</v>
       </c>
@@ -2636,7 +2638,7 @@
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22">
       <c r="A22" s="2" t="s">
         <v>82</v>
       </c>
@@ -2653,7 +2655,7 @@
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23">
       <c r="A23" s="2" t="s">
         <v>86</v>
       </c>
@@ -2670,7 +2672,7 @@
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24">
       <c r="A24" s="2" t="s">
         <v>90</v>
       </c>
@@ -2687,7 +2689,7 @@
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25">
       <c r="A25" s="2" t="s">
         <v>94</v>
       </c>
@@ -2703,7 +2705,7 @@
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26">
       <c r="A26" s="2" t="s">
         <v>98</v>
       </c>
@@ -2719,7 +2721,7 @@
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27">
       <c r="A27" s="2" t="s">
         <v>102</v>
       </c>
@@ -2736,7 +2738,7 @@
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -2751,11 +2753,12 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D4:D24">
     <sortCondition ref="D4:D24"/>
   </sortState>
-  <mergeCells count="1">
+  <mergeCells>
     <mergeCell ref="A1:I2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -2767,16 +2770,16 @@
   <dimension ref="A1:AN27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection activeCell="A4" sqref="A4:G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="1" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" bestFit="1" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" s="22" t="s">
         <v>156</v>
       </c>
@@ -2787,7 +2790,7 @@
       <c r="F1" s="22"/>
       <c r="G1" s="22"/>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="2">
       <c r="A2" s="23"/>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
@@ -2796,687 +2799,688 @@
       <c r="F2" s="23"/>
       <c r="G2" s="23"/>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="3">
       <c r="A3" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="K3" t="s">
+      <c r="K3" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="L3" t="s">
+      <c r="L3" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="N3" t="s">
+      <c r="N3" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="O3" t="s">
+      <c r="O3" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="P3" t="s">
+      <c r="P3" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="Q3" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="R3" t="s">
+      <c r="R3" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="S3" t="s">
+      <c r="S3" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="T3" t="s">
+      <c r="T3" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="U3" t="s">
+      <c r="U3" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="V3" t="s">
+      <c r="V3" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="W3" t="s">
+      <c r="W3" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="X3" t="s">
+      <c r="X3" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Y3" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="Z3" s="0" t="s">
         <v>114</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AA3" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AB3" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AC3" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AD3" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AE3" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="AF3" t="s">
+      <c r="AF3" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="AG3" t="s">
+      <c r="AG3" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="AH3" t="s">
+      <c r="AH3" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="AI3" t="s">
+      <c r="AI3" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="AJ3" t="s">
+      <c r="AJ3" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="AK3" t="s">
+      <c r="AK3" s="0" t="s">
         <v>139</v>
       </c>
-      <c r="AL3" t="s">
+      <c r="AL3" s="0" t="s">
         <v>141</v>
       </c>
-      <c r="AM3" t="s">
+      <c r="AM3" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="AN3" t="s">
+      <c r="AN3" s="0" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4">
+      <c r="A4" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="0">
         <v>67</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="0">
         <v>66</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="0">
         <v>85</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="0">
         <v>49</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="0">
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5">
+      <c r="A5" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="0">
         <v>61</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="0">
         <v>75</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="0">
         <v>68</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="0">
         <v>63</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="0">
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6">
+      <c r="A6" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="0">
         <v>69</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="0">
         <v>76</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="0">
         <v>76</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="0">
         <v>51</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="0">
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7">
+      <c r="A7" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="0">
         <v>70</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="0">
         <v>78</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="0">
         <v>74</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="0">
         <v>60</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="0">
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8">
+      <c r="A8" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="0">
         <v>75</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="0">
         <v>69</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="0">
         <v>73</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="0">
         <v>33</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="0">
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9">
+      <c r="A9" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="0">
         <v>45</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="0">
         <v>73</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="0">
         <v>78</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="0">
         <v>50</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="0">
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10">
+      <c r="A10" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="0">
         <v>64</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="0">
         <v>41</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="0">
         <v>40</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="0">
         <v>50</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="0">
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11">
+      <c r="A11" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="0">
         <v>67</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="0">
         <v>71</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="0">
         <v>64</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="0">
         <v>52</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="0">
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12">
+      <c r="A12" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="0">
         <v>48</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="0">
         <v>76</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="0">
         <v>62</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="0">
         <v>86</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="0">
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13">
+      <c r="A13" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="0">
         <v>57</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="0">
         <v>62</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="0">
         <v>71</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="0">
         <v>48</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="0">
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14">
+      <c r="A14" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="0">
         <v>84</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="0">
         <v>53</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="0">
         <v>85</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="0">
         <v>37</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="0">
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15">
+      <c r="A15" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="0">
         <v>55</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="0">
         <v>33</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="0">
         <v>69</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="0">
         <v>65</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="0">
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="16">
+      <c r="A16" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="0">
         <v>75</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="0">
         <v>98</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="0">
         <v>69</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="0">
         <v>59</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="0">
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="17">
+      <c r="A17" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="0">
         <v>79</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="0">
         <v>79</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="0">
         <v>73</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="0">
         <v>60</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="0">
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="18">
+      <c r="A18" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="0">
         <v>53</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="0">
         <v>73</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="0">
         <v>75</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="0">
         <v>40</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="0">
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="19">
+      <c r="A19" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="0">
         <v>68</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="0">
         <v>82</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="0">
         <v>66</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="0">
         <v>53</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="0">
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="20">
+      <c r="A20" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="0" t="s">
         <v>75</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="0">
         <v>76</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="0">
         <v>74</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="0">
         <v>69</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="0">
         <v>56</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="0">
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="21">
+      <c r="A21" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="0">
         <v>42</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="0">
         <v>68</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="0">
         <v>68</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="0">
         <v>61</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="0">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="22">
+      <c r="A22" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="0">
         <v>60</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="0">
         <v>81</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="0">
         <v>71</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="0">
         <v>45</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="0">
         <v>67</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="23">
+      <c r="A23" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="0">
         <v>81</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="0">
         <v>71</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="0">
         <v>85</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="0">
         <v>48</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="0">
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="24">
+      <c r="A24" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="0">
         <v>72</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="0">
         <v>77</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="0">
         <v>95</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="0">
         <v>40</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="0">
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="25">
+      <c r="A25" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="0">
         <v>62</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="0">
         <v>45</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="0">
         <v>38</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="0">
         <v>38</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="0">
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="26">
+      <c r="A26" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="0">
         <v>54</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="0">
         <v>78</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="0">
         <v>84</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="0">
         <v>56</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="0">
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="27">
+      <c r="A27" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="0">
         <v>48</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="0">
         <v>90</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="0">
         <v>89</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="0">
         <v>53</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="0">
         <v>75</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells>
     <mergeCell ref="A1:G2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0"/>
+  <headerFooter/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
@@ -3494,10 +3498,10 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.140625" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" bestFit="1" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" s="24" t="s">
         <v>158</v>
       </c>
@@ -3506,147 +3510,147 @@
       <c r="D1" s="24"/>
       <c r="E1" s="24"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2">
       <c r="A2" s="24"/>
       <c r="B2" s="24"/>
       <c r="C2" s="24"/>
       <c r="D2" s="24"/>
       <c r="E2" s="24"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3">
+      <c r="A3" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>161</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="0">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4">
       <c r="A4" s="5" t="s">
         <v>163</v>
       </c>
       <c r="B4" s="7">
         <v>125</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="0">
         <f>B4*F3</f>
         <v>4750</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="0" t="s">
         <v>164</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="0">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5">
       <c r="A5" s="5" t="s">
         <v>165</v>
       </c>
       <c r="B5" s="7">
         <v>250</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="0">
         <f>B5*F4</f>
         <v>2500</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="0">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" ht="30">
       <c r="A6" s="5" t="s">
         <v>167</v>
       </c>
       <c r="B6" s="7">
         <v>200</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="0">
         <f>B6*F5</f>
         <v>600</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7">
       <c r="A7" s="5" t="s">
         <v>168</v>
       </c>
       <c r="B7" s="7">
         <v>500</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="0">
         <v>500</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" ht="30">
       <c r="A8" s="5" t="s">
         <v>169</v>
       </c>
       <c r="B8" s="6">
         <v>800</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="0">
         <f>B8*2</f>
         <v>1600</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9">
       <c r="A9" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="0">
         <v>400</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="0">
         <v>400</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10">
       <c r="A10" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="0">
         <v>600</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="0">
         <v>600</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11">
       <c r="A11" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="0">
         <v>1000</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="0">
         <v>1000</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12">
       <c r="A12" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="0">
         <v>100</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="0">
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13">
+      <c r="A13" s="0" t="s">
         <v>174</v>
       </c>
       <c r="C13" s="8">
@@ -3654,25 +3658,25 @@
         <v>12050</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14">
+      <c r="A14" s="0" t="s">
         <v>175</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="0">
         <v>12000</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="0">
         <f>C14-C13</f>
         <v>-50</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16">
       <c r="A16" s="25" t="s">
         <v>176</v>
       </c>
       <c r="B16" s="25"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17">
       <c r="A17" s="9" t="s">
         <v>163</v>
       </c>
@@ -3680,7 +3684,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18">
       <c r="A18" s="9" t="s">
         <v>165</v>
       </c>
@@ -3688,7 +3692,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" ht="30">
       <c r="A19" s="9" t="s">
         <v>167</v>
       </c>
@@ -3696,7 +3700,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20">
       <c r="A20" s="9" t="s">
         <v>168</v>
       </c>
@@ -3704,7 +3708,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" ht="30">
       <c r="A21" s="9" t="s">
         <v>180</v>
       </c>
@@ -3712,7 +3716,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22">
       <c r="A22" s="9" t="s">
         <v>170</v>
       </c>
@@ -3720,7 +3724,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23">
       <c r="A23" s="9" t="s">
         <v>171</v>
       </c>
@@ -3728,7 +3732,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24">
       <c r="A24" s="9" t="s">
         <v>172</v>
       </c>
@@ -3737,10 +3741,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells>
     <mergeCell ref="A1:E2"/>
     <mergeCell ref="A16:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added support for both my OSes
</commit_message>
<xml_diff>
--- a/FPL Luster totaloversikt.xlsx
+++ b/FPL Luster totaloversikt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\FantasyLeaguePointsFetcher\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project\fpl\FantasyLeaguePointsFetcher\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7945845D-A565-4029-AE22-3CC40200443E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CE389EF-8775-4B6F-B972-A47E3A2255CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{9393CECB-8678-4F9E-A49E-EF671E63BC0A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{9393CECB-8678-4F9E-A49E-EF671E63BC0A}"/>
   </bookViews>
   <sheets>
     <sheet name="GW oversikt" sheetId="2" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="189">
   <si>
     <t>Luster FPL oversikt</t>
   </si>
@@ -1283,7 +1283,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8EE5AE49-73B7-B443-9AC9-E3CB9F929E8A}" name="Tabell1" displayName="Tabell1" ref="A3:AO27" totalsRowShown="0">
   <autoFilter ref="A3:AO27" xr:uid="{8EE5AE49-73B7-B443-9AC9-E3CB9F929E8A}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:AO27">
-    <sortCondition descending="1" ref="AC3:AC27"/>
+    <sortCondition descending="1" ref="AE3:AE27"/>
   </sortState>
   <tableColumns count="41">
     <tableColumn id="1" xr3:uid="{74CEA007-FA61-3D40-A38E-5915AED44115}" name="Lagnamn" dataDxfId="9" dataCellStyle="Totalt"/>
@@ -1673,8 +1673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43A5FFB2-DF08-474B-9B68-3293440C8632}">
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2412,7 +2412,9 @@
       <c r="B38" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="C38" s="14"/>
+      <c r="C38" s="14" t="s">
+        <v>39</v>
+      </c>
       <c r="D38" s="14"/>
       <c r="E38" s="14"/>
       <c r="F38" s="14"/>
@@ -2425,7 +2427,9 @@
       <c r="B39" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="C39" s="14"/>
+      <c r="C39" s="14" t="s">
+        <v>24</v>
+      </c>
       <c r="D39" s="14"/>
       <c r="E39" s="14"/>
       <c r="F39" s="14"/>
@@ -2438,7 +2442,9 @@
       <c r="D40" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="E40" s="18"/>
+      <c r="E40" s="24" t="s">
+        <v>24</v>
+      </c>
       <c r="F40" s="18"/>
       <c r="G40" s="18"/>
     </row>
@@ -3100,8 +3106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{909B07EA-687F-744F-B9DD-893A1ABB287D}">
   <dimension ref="A1:AO57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AD1" sqref="AD1:AD1048576"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3264,95 +3270,101 @@
     </row>
     <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4">
+        <v>69</v>
+      </c>
+      <c r="D4">
+        <v>76</v>
+      </c>
+      <c r="E4">
+        <v>76</v>
+      </c>
+      <c r="F4">
+        <v>51</v>
+      </c>
+      <c r="G4">
+        <v>82</v>
+      </c>
+      <c r="H4">
+        <v>49</v>
+      </c>
+      <c r="I4">
+        <v>48</v>
+      </c>
+      <c r="J4">
+        <v>20</v>
+      </c>
+      <c r="K4">
         <v>64</v>
       </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4">
+      <c r="L4">
+        <v>45</v>
+      </c>
+      <c r="M4">
+        <v>51</v>
+      </c>
+      <c r="N4">
+        <v>54</v>
+      </c>
+      <c r="O4">
         <v>75</v>
       </c>
-      <c r="D4">
-        <v>98</v>
-      </c>
-      <c r="E4">
-        <v>69</v>
-      </c>
-      <c r="F4">
-        <v>59</v>
-      </c>
-      <c r="G4">
-        <v>56</v>
-      </c>
-      <c r="H4">
+      <c r="P4">
         <v>57</v>
       </c>
-      <c r="I4">
-        <v>55</v>
-      </c>
-      <c r="J4">
-        <v>56</v>
-      </c>
-      <c r="K4">
-        <v>67</v>
-      </c>
-      <c r="L4">
-        <v>48</v>
-      </c>
-      <c r="M4">
-        <v>31</v>
-      </c>
-      <c r="N4">
-        <v>52</v>
-      </c>
-      <c r="O4">
-        <v>64</v>
-      </c>
-      <c r="P4">
-        <v>62</v>
-      </c>
       <c r="Q4">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="R4">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="S4">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="T4">
         <v>62</v>
       </c>
       <c r="U4">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="V4">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="W4">
-        <v>60</v>
+        <v>91</v>
       </c>
       <c r="X4">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="Y4">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="Z4">
-        <v>93</v>
+        <v>145</v>
       </c>
       <c r="AA4">
-        <v>95</v>
+        <v>112</v>
       </c>
       <c r="AB4">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="AC4">
-        <v>84</v>
+        <v>63</v>
+      </c>
+      <c r="AD4">
+        <v>71</v>
+      </c>
+      <c r="AE4">
+        <v>67</v>
       </c>
       <c r="AO4">
         <f>SUM(Tabell1[[#This Row],[GW1]:[GW38]])</f>
-        <v>1794</v>
+        <v>1962</v>
       </c>
     </row>
     <row r="5" spans="1:41" x14ac:dyDescent="0.25">
@@ -3441,604 +3453,646 @@
         <v>86</v>
       </c>
       <c r="AC5">
-        <v>70</v>
+        <v>72</v>
+      </c>
+      <c r="AD5">
+        <v>59</v>
+      </c>
+      <c r="AE5">
+        <v>64</v>
       </c>
       <c r="AO5">
         <f>SUM(Tabell1[[#This Row],[GW1]:[GW38]])</f>
-        <v>1809</v>
+        <v>1934</v>
       </c>
     </row>
     <row r="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C6">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D6">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="E6">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="F6">
+        <v>86</v>
+      </c>
+      <c r="G6">
+        <v>45</v>
+      </c>
+      <c r="H6">
+        <v>37</v>
+      </c>
+      <c r="I6">
+        <v>20</v>
+      </c>
+      <c r="J6">
+        <v>33</v>
+      </c>
+      <c r="K6">
+        <v>26</v>
+      </c>
+      <c r="L6">
+        <v>46</v>
+      </c>
+      <c r="M6">
+        <v>50</v>
+      </c>
+      <c r="N6">
         <v>40</v>
       </c>
-      <c r="G6">
-        <v>51</v>
-      </c>
-      <c r="H6">
-        <v>75</v>
-      </c>
-      <c r="I6">
+      <c r="O6">
+        <v>44</v>
+      </c>
+      <c r="P6">
         <v>42</v>
       </c>
-      <c r="J6">
-        <v>56</v>
-      </c>
-      <c r="K6">
+      <c r="Q6">
+        <v>48</v>
+      </c>
+      <c r="R6">
+        <v>45</v>
+      </c>
+      <c r="S6">
+        <v>24</v>
+      </c>
+      <c r="T6">
+        <v>30</v>
+      </c>
+      <c r="U6">
         <v>55</v>
       </c>
-      <c r="L6">
+      <c r="V6">
+        <v>61</v>
+      </c>
+      <c r="W6">
+        <v>43</v>
+      </c>
+      <c r="X6">
+        <v>47</v>
+      </c>
+      <c r="Y6">
+        <v>54</v>
+      </c>
+      <c r="Z6">
+        <v>44</v>
+      </c>
+      <c r="AA6">
+        <v>57</v>
+      </c>
+      <c r="AB6">
+        <v>41</v>
+      </c>
+      <c r="AC6">
         <v>52</v>
       </c>
-      <c r="M6">
-        <v>45</v>
-      </c>
-      <c r="N6">
-        <v>82</v>
-      </c>
-      <c r="O6">
-        <v>72</v>
-      </c>
-      <c r="P6">
-        <v>92</v>
-      </c>
-      <c r="Q6">
-        <v>73</v>
-      </c>
-      <c r="R6">
-        <v>41</v>
-      </c>
-      <c r="S6">
-        <v>62</v>
-      </c>
-      <c r="T6">
-        <v>60</v>
-      </c>
-      <c r="U6">
-        <v>82</v>
-      </c>
-      <c r="V6">
-        <v>54</v>
-      </c>
-      <c r="W6">
-        <v>44</v>
-      </c>
-      <c r="X6">
-        <v>53</v>
-      </c>
-      <c r="Y6">
-        <v>65</v>
-      </c>
-      <c r="Z6">
-        <v>127</v>
-      </c>
-      <c r="AA6">
-        <v>105</v>
-      </c>
-      <c r="AB6">
-        <v>66</v>
-      </c>
-      <c r="AC6">
-        <v>69</v>
+      <c r="AD6">
+        <v>43</v>
+      </c>
+      <c r="AE6">
+        <v>64</v>
       </c>
       <c r="AO6">
         <f>SUM(Tabell1[[#This Row],[GW1]:[GW38]])</f>
-        <v>1764</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B7" t="s">
-        <v>68</v>
+        <v>12</v>
       </c>
       <c r="C7">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="D7">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="E7">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="F7">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="G7">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="H7">
-        <v>35</v>
+        <v>62</v>
       </c>
       <c r="I7">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="J7">
         <v>32</v>
       </c>
       <c r="K7">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="L7">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M7">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="N7">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="O7">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="P7">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="Q7">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="R7">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="S7">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="T7">
+        <v>56</v>
+      </c>
+      <c r="U7">
+        <v>55</v>
+      </c>
+      <c r="V7">
+        <v>71</v>
+      </c>
+      <c r="W7">
         <v>70</v>
       </c>
-      <c r="U7">
-        <v>72</v>
-      </c>
-      <c r="V7">
-        <v>56</v>
-      </c>
-      <c r="W7">
-        <v>79</v>
-      </c>
       <c r="X7">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="Y7">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="Z7">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="AA7">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="AB7">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="AC7">
+        <v>55</v>
+      </c>
+      <c r="AD7">
+        <v>63</v>
+      </c>
+      <c r="AE7">
         <v>61</v>
       </c>
       <c r="AO7">
         <f>SUM(Tabell1[[#This Row],[GW1]:[GW38]])</f>
-        <v>1765</v>
+        <v>1844</v>
       </c>
     </row>
     <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="C8">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="D8">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E8">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F8">
+        <v>40</v>
+      </c>
+      <c r="G8">
         <v>51</v>
       </c>
-      <c r="G8">
+      <c r="H8">
+        <v>75</v>
+      </c>
+      <c r="I8">
+        <v>42</v>
+      </c>
+      <c r="J8">
+        <v>56</v>
+      </c>
+      <c r="K8">
+        <v>55</v>
+      </c>
+      <c r="L8">
+        <v>52</v>
+      </c>
+      <c r="M8">
+        <v>45</v>
+      </c>
+      <c r="N8">
         <v>82</v>
       </c>
-      <c r="H8">
-        <v>49</v>
-      </c>
-      <c r="I8">
-        <v>48</v>
-      </c>
-      <c r="J8">
-        <v>20</v>
-      </c>
-      <c r="K8">
-        <v>64</v>
-      </c>
-      <c r="L8">
-        <v>45</v>
-      </c>
-      <c r="M8">
-        <v>51</v>
-      </c>
-      <c r="N8">
+      <c r="O8">
+        <v>72</v>
+      </c>
+      <c r="P8">
+        <v>92</v>
+      </c>
+      <c r="Q8">
+        <v>73</v>
+      </c>
+      <c r="R8">
+        <v>41</v>
+      </c>
+      <c r="S8">
+        <v>62</v>
+      </c>
+      <c r="T8">
+        <v>60</v>
+      </c>
+      <c r="U8">
+        <v>82</v>
+      </c>
+      <c r="V8">
         <v>54</v>
       </c>
-      <c r="O8">
+      <c r="W8">
+        <v>44</v>
+      </c>
+      <c r="X8">
+        <v>53</v>
+      </c>
+      <c r="Y8">
+        <v>65</v>
+      </c>
+      <c r="Z8">
+        <v>127</v>
+      </c>
+      <c r="AA8">
+        <v>105</v>
+      </c>
+      <c r="AB8">
+        <v>66</v>
+      </c>
+      <c r="AC8">
+        <v>68</v>
+      </c>
+      <c r="AD8">
         <v>75</v>
       </c>
-      <c r="P8">
-        <v>57</v>
-      </c>
-      <c r="Q8">
-        <v>57</v>
-      </c>
-      <c r="R8">
-        <v>66</v>
-      </c>
-      <c r="S8">
-        <v>83</v>
-      </c>
-      <c r="T8">
-        <v>62</v>
-      </c>
-      <c r="U8">
-        <v>88</v>
-      </c>
-      <c r="V8">
-        <v>63</v>
-      </c>
-      <c r="W8">
-        <v>91</v>
-      </c>
-      <c r="X8">
-        <v>45</v>
-      </c>
-      <c r="Y8">
-        <v>69</v>
-      </c>
-      <c r="Z8">
-        <v>145</v>
-      </c>
-      <c r="AA8">
-        <v>112</v>
-      </c>
-      <c r="AB8">
-        <v>63</v>
-      </c>
-      <c r="AC8">
-        <v>61</v>
+      <c r="AE8">
+        <v>60</v>
       </c>
       <c r="AO8">
         <f>SUM(Tabell1[[#This Row],[GW1]:[GW38]])</f>
-        <v>1822</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>89</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C9">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="D9">
+        <v>77</v>
+      </c>
+      <c r="E9">
+        <v>95</v>
+      </c>
+      <c r="F9">
+        <v>40</v>
+      </c>
+      <c r="G9">
+        <v>61</v>
+      </c>
+      <c r="H9">
+        <v>45</v>
+      </c>
+      <c r="I9">
+        <v>42</v>
+      </c>
+      <c r="J9">
+        <v>53</v>
+      </c>
+      <c r="K9">
         <v>69</v>
       </c>
-      <c r="E9">
-        <v>73</v>
-      </c>
-      <c r="F9">
-        <v>33</v>
-      </c>
-      <c r="G9">
-        <v>39</v>
-      </c>
-      <c r="H9">
-        <v>62</v>
-      </c>
-      <c r="I9">
+      <c r="L9">
+        <v>38</v>
+      </c>
+      <c r="M9">
+        <v>64</v>
+      </c>
+      <c r="N9">
+        <v>57</v>
+      </c>
+      <c r="O9">
+        <v>43</v>
+      </c>
+      <c r="P9">
+        <v>92</v>
+      </c>
+      <c r="Q9">
+        <v>59</v>
+      </c>
+      <c r="R9">
+        <v>77</v>
+      </c>
+      <c r="S9">
+        <v>76</v>
+      </c>
+      <c r="T9">
+        <v>70</v>
+      </c>
+      <c r="U9">
+        <v>80</v>
+      </c>
+      <c r="V9">
         <v>74</v>
       </c>
-      <c r="J9">
-        <v>28</v>
-      </c>
-      <c r="K9">
-        <v>56</v>
-      </c>
-      <c r="L9">
-        <v>34</v>
-      </c>
-      <c r="M9">
-        <v>39</v>
-      </c>
-      <c r="N9">
+      <c r="W9">
         <v>52</v>
       </c>
-      <c r="O9">
-        <v>77</v>
-      </c>
-      <c r="P9">
-        <v>62</v>
-      </c>
-      <c r="Q9">
-        <v>38</v>
-      </c>
-      <c r="R9">
-        <v>43</v>
-      </c>
-      <c r="S9">
-        <v>77</v>
-      </c>
-      <c r="T9">
-        <v>52</v>
-      </c>
-      <c r="U9">
-        <v>69</v>
-      </c>
-      <c r="V9">
+      <c r="X9">
+        <v>36</v>
+      </c>
+      <c r="Y9">
+        <v>59</v>
+      </c>
+      <c r="Z9">
+        <v>131</v>
+      </c>
+      <c r="AA9">
+        <v>87</v>
+      </c>
+      <c r="AB9">
+        <v>89</v>
+      </c>
+      <c r="AC9">
         <v>57</v>
       </c>
-      <c r="W9">
-        <v>81</v>
-      </c>
-      <c r="X9">
-        <v>57</v>
-      </c>
-      <c r="Y9">
-        <v>70</v>
-      </c>
-      <c r="Z9">
-        <v>142</v>
-      </c>
-      <c r="AA9">
-        <v>107</v>
-      </c>
-      <c r="AB9">
-        <v>67</v>
-      </c>
-      <c r="AC9">
-        <v>58</v>
+      <c r="AD9">
+        <v>65</v>
+      </c>
+      <c r="AE9">
+        <v>60</v>
       </c>
       <c r="AO9">
         <f>SUM(Tabell1[[#This Row],[GW1]:[GW38]])</f>
-        <v>1691</v>
+        <v>1920</v>
       </c>
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>59</v>
       </c>
       <c r="C10">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="D10">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E10">
         <v>85</v>
       </c>
       <c r="F10">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G10">
+        <v>61</v>
+      </c>
+      <c r="H10">
+        <v>68</v>
+      </c>
+      <c r="I10">
+        <v>71</v>
+      </c>
+      <c r="J10">
+        <v>48</v>
+      </c>
+      <c r="K10">
+        <v>70</v>
+      </c>
+      <c r="L10">
+        <v>38</v>
+      </c>
+      <c r="M10">
         <v>66</v>
       </c>
-      <c r="H10">
-        <v>58</v>
-      </c>
-      <c r="I10">
+      <c r="N10">
+        <v>42</v>
+      </c>
+      <c r="O10">
+        <v>62</v>
+      </c>
+      <c r="P10">
+        <v>55</v>
+      </c>
+      <c r="Q10">
+        <v>52</v>
+      </c>
+      <c r="R10">
+        <v>82</v>
+      </c>
+      <c r="S10">
+        <v>53</v>
+      </c>
+      <c r="T10">
+        <v>61</v>
+      </c>
+      <c r="U10">
+        <v>87</v>
+      </c>
+      <c r="V10">
+        <v>52</v>
+      </c>
+      <c r="W10">
+        <v>91</v>
+      </c>
+      <c r="X10">
+        <v>47</v>
+      </c>
+      <c r="Y10">
+        <v>73</v>
+      </c>
+      <c r="Z10">
+        <v>136</v>
+      </c>
+      <c r="AA10">
+        <v>91</v>
+      </c>
+      <c r="AB10">
+        <v>79</v>
+      </c>
+      <c r="AC10">
+        <v>42</v>
+      </c>
+      <c r="AD10">
         <v>50</v>
       </c>
-      <c r="J10">
-        <v>51</v>
-      </c>
-      <c r="K10">
-        <v>60</v>
-      </c>
-      <c r="L10">
-        <v>51</v>
-      </c>
-      <c r="M10">
-        <v>69</v>
-      </c>
-      <c r="N10">
-        <v>63</v>
-      </c>
-      <c r="O10">
-        <v>79</v>
-      </c>
-      <c r="P10">
-        <v>63</v>
-      </c>
-      <c r="Q10">
-        <v>61</v>
-      </c>
-      <c r="R10">
-        <v>47</v>
-      </c>
-      <c r="S10">
-        <v>80</v>
-      </c>
-      <c r="T10">
-        <v>53</v>
-      </c>
-      <c r="U10">
-        <v>94</v>
-      </c>
-      <c r="V10">
-        <v>50</v>
-      </c>
-      <c r="W10">
-        <v>80</v>
-      </c>
-      <c r="X10">
-        <v>68</v>
-      </c>
-      <c r="Y10">
-        <v>69</v>
-      </c>
-      <c r="Z10">
-        <v>128</v>
-      </c>
-      <c r="AA10">
-        <v>102</v>
-      </c>
-      <c r="AB10">
-        <v>89</v>
-      </c>
-      <c r="AC10">
-        <v>56</v>
+      <c r="AE10">
+        <v>59</v>
       </c>
       <c r="AO10">
         <f>SUM(Tabell1[[#This Row],[GW1]:[GW38]])</f>
-        <v>1854</v>
+        <v>1921</v>
       </c>
     </row>
     <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11">
+        <v>67</v>
+      </c>
+      <c r="D11">
+        <v>71</v>
+      </c>
+      <c r="E11">
+        <v>64</v>
+      </c>
+      <c r="F11">
+        <v>52</v>
+      </c>
+      <c r="G11">
+        <v>65</v>
+      </c>
+      <c r="H11">
+        <v>61</v>
+      </c>
+      <c r="I11">
+        <v>58</v>
+      </c>
+      <c r="J11">
+        <v>31</v>
+      </c>
+      <c r="K11">
+        <v>31</v>
+      </c>
+      <c r="L11">
         <v>57</v>
       </c>
-      <c r="B11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11">
-        <v>84</v>
-      </c>
-      <c r="D11">
-        <v>53</v>
-      </c>
-      <c r="E11">
-        <v>85</v>
-      </c>
-      <c r="F11">
-        <v>37</v>
-      </c>
-      <c r="G11">
-        <v>69</v>
-      </c>
-      <c r="H11">
-        <v>62</v>
-      </c>
-      <c r="I11">
-        <v>43</v>
-      </c>
-      <c r="J11">
-        <v>32</v>
-      </c>
-      <c r="K11">
+      <c r="M11">
+        <v>81</v>
+      </c>
+      <c r="N11">
+        <v>54</v>
+      </c>
+      <c r="O11">
+        <v>55</v>
+      </c>
+      <c r="P11">
         <v>74</v>
       </c>
-      <c r="L11">
-        <v>30</v>
-      </c>
-      <c r="M11">
-        <v>72</v>
-      </c>
-      <c r="N11">
-        <v>51</v>
-      </c>
-      <c r="O11">
-        <v>93</v>
-      </c>
-      <c r="P11">
-        <v>51</v>
-      </c>
       <c r="Q11">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="R11">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="S11">
-        <v>67</v>
+        <v>103</v>
       </c>
       <c r="T11">
-        <v>56</v>
+        <v>74</v>
       </c>
       <c r="U11">
-        <v>55</v>
+        <v>73</v>
       </c>
       <c r="V11">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="W11">
-        <v>70</v>
+        <v>98</v>
       </c>
       <c r="X11">
         <v>42</v>
       </c>
       <c r="Y11">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="Z11">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="AA11">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AB11">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="AC11">
-        <v>56</v>
+        <v>49</v>
+      </c>
+      <c r="AD11">
+        <v>59</v>
+      </c>
+      <c r="AE11">
+        <v>58</v>
       </c>
       <c r="AO11">
         <f>SUM(Tabell1[[#This Row],[GW1]:[GW38]])</f>
-        <v>1721</v>
+        <v>1921</v>
       </c>
     </row>
     <row r="12" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>103</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>104</v>
+        <v>32</v>
       </c>
       <c r="C12">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="D12">
-        <v>90</v>
+        <v>69</v>
       </c>
       <c r="E12">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="F12">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="G12">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="H12">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="I12">
-        <v>48</v>
+        <v>74</v>
       </c>
       <c r="J12">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="K12">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="L12">
         <v>34</v>
@@ -4047,1079 +4101,1151 @@
         <v>39</v>
       </c>
       <c r="N12">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="O12">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="P12">
+        <v>62</v>
+      </c>
+      <c r="Q12">
+        <v>38</v>
+      </c>
+      <c r="R12">
+        <v>43</v>
+      </c>
+      <c r="S12">
         <v>77</v>
       </c>
-      <c r="Q12">
-        <v>56</v>
-      </c>
-      <c r="R12">
-        <v>47</v>
-      </c>
-      <c r="S12">
+      <c r="T12">
+        <v>52</v>
+      </c>
+      <c r="U12">
+        <v>69</v>
+      </c>
+      <c r="V12">
         <v>57</v>
       </c>
-      <c r="T12">
-        <v>54</v>
-      </c>
-      <c r="U12">
-        <v>75</v>
-      </c>
-      <c r="V12">
-        <v>59</v>
-      </c>
       <c r="W12">
-        <v>50</v>
+        <v>81</v>
       </c>
       <c r="X12">
-        <v>31</v>
+        <v>57</v>
       </c>
       <c r="Y12">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="Z12">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="AA12">
-        <v>84</v>
+        <v>107</v>
       </c>
       <c r="AB12">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="AC12">
+        <v>64</v>
+      </c>
+      <c r="AD12">
+        <v>74</v>
+      </c>
+      <c r="AE12">
         <v>55</v>
       </c>
       <c r="AO12">
         <f>SUM(Tabell1[[#This Row],[GW1]:[GW38]])</f>
-        <v>1610</v>
+        <v>1826</v>
       </c>
     </row>
     <row r="13" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="B13" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C13">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D13">
+        <v>78</v>
+      </c>
+      <c r="E13">
+        <v>84</v>
+      </c>
+      <c r="F13">
+        <v>56</v>
+      </c>
+      <c r="G13">
+        <v>63</v>
+      </c>
+      <c r="H13">
+        <v>34</v>
+      </c>
+      <c r="I13">
+        <v>54</v>
+      </c>
+      <c r="J13">
+        <v>25</v>
+      </c>
+      <c r="K13">
+        <v>68</v>
+      </c>
+      <c r="L13">
+        <v>38</v>
+      </c>
+      <c r="M13">
+        <v>56</v>
+      </c>
+      <c r="N13">
         <v>45</v>
       </c>
-      <c r="E13">
-        <v>38</v>
-      </c>
-      <c r="F13">
-        <v>38</v>
-      </c>
-      <c r="G13">
-        <v>35</v>
-      </c>
-      <c r="H13">
-        <v>62</v>
-      </c>
-      <c r="I13">
-        <v>46</v>
-      </c>
-      <c r="J13">
-        <v>26</v>
-      </c>
-      <c r="K13">
-        <v>55</v>
-      </c>
-      <c r="L13">
-        <v>29</v>
-      </c>
-      <c r="M13">
-        <v>51</v>
-      </c>
-      <c r="N13">
-        <v>32</v>
-      </c>
       <c r="O13">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="P13">
         <v>44</v>
       </c>
       <c r="Q13">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="R13">
         <v>43</v>
       </c>
       <c r="S13">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="T13">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="U13">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="V13">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="W13">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="X13">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="Y13">
+        <v>62</v>
+      </c>
+      <c r="Z13">
+        <v>103</v>
+      </c>
+      <c r="AA13">
         <v>64</v>
       </c>
-      <c r="Z13">
-        <v>69</v>
-      </c>
-      <c r="AA13">
-        <v>57</v>
-      </c>
       <c r="AB13">
-        <v>34</v>
+        <v>74</v>
       </c>
       <c r="AC13">
+        <v>45</v>
+      </c>
+      <c r="AD13">
+        <v>55</v>
+      </c>
+      <c r="AE13">
         <v>55</v>
       </c>
       <c r="AO13">
         <f>SUM(Tabell1[[#This Row],[GW1]:[GW38]])</f>
-        <v>1278</v>
+        <v>1620</v>
       </c>
     </row>
     <row r="14" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14">
+        <v>68</v>
+      </c>
+      <c r="D14">
+        <v>82</v>
+      </c>
+      <c r="E14">
+        <v>66</v>
+      </c>
+      <c r="F14">
+        <v>53</v>
+      </c>
+      <c r="G14">
+        <v>77</v>
+      </c>
+      <c r="H14">
+        <v>42</v>
+      </c>
+      <c r="I14">
+        <v>59</v>
+      </c>
+      <c r="J14">
+        <v>35</v>
+      </c>
+      <c r="K14">
         <v>48</v>
       </c>
-      <c r="B14" t="s">
+      <c r="L14">
         <v>30</v>
       </c>
-      <c r="C14">
-        <v>48</v>
-      </c>
-      <c r="D14">
+      <c r="M14">
+        <v>35</v>
+      </c>
+      <c r="N14">
+        <v>62</v>
+      </c>
+      <c r="O14">
+        <v>64</v>
+      </c>
+      <c r="P14">
         <v>76</v>
       </c>
-      <c r="E14">
-        <v>62</v>
-      </c>
-      <c r="F14">
-        <v>86</v>
-      </c>
-      <c r="G14">
-        <v>45</v>
-      </c>
-      <c r="H14">
-        <v>37</v>
-      </c>
-      <c r="I14">
-        <v>20</v>
-      </c>
-      <c r="J14">
-        <v>33</v>
-      </c>
-      <c r="K14">
-        <v>26</v>
-      </c>
-      <c r="L14">
-        <v>46</v>
-      </c>
-      <c r="M14">
-        <v>50</v>
-      </c>
-      <c r="N14">
-        <v>40</v>
-      </c>
-      <c r="O14">
-        <v>44</v>
-      </c>
-      <c r="P14">
-        <v>42</v>
-      </c>
       <c r="Q14">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="R14">
         <v>45</v>
       </c>
       <c r="S14">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="T14">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="U14">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="V14">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="W14">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="X14">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="Y14">
+        <v>57</v>
+      </c>
+      <c r="Z14">
+        <v>122</v>
+      </c>
+      <c r="AA14">
+        <v>108</v>
+      </c>
+      <c r="AB14">
+        <v>66</v>
+      </c>
+      <c r="AC14">
+        <v>57</v>
+      </c>
+      <c r="AD14">
+        <v>63</v>
+      </c>
+      <c r="AE14">
         <v>54</v>
-      </c>
-      <c r="Z14">
-        <v>44</v>
-      </c>
-      <c r="AA14">
-        <v>57</v>
-      </c>
-      <c r="AB14">
-        <v>41</v>
-      </c>
-      <c r="AC14">
-        <v>53</v>
       </c>
       <c r="AO14">
         <f>SUM(Tabell1[[#This Row],[GW1]:[GW38]])</f>
-        <v>1257</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="15" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C15">
+        <v>67</v>
+      </c>
+      <c r="D15">
+        <v>66</v>
+      </c>
+      <c r="E15">
+        <v>85</v>
+      </c>
+      <c r="F15">
+        <v>49</v>
+      </c>
+      <c r="G15">
+        <v>66</v>
+      </c>
+      <c r="H15">
+        <v>58</v>
+      </c>
+      <c r="I15">
+        <v>50</v>
+      </c>
+      <c r="J15">
+        <v>51</v>
+      </c>
+      <c r="K15">
+        <v>60</v>
+      </c>
+      <c r="L15">
+        <v>51</v>
+      </c>
+      <c r="M15">
+        <v>69</v>
+      </c>
+      <c r="N15">
+        <v>63</v>
+      </c>
+      <c r="O15">
+        <v>79</v>
+      </c>
+      <c r="P15">
+        <v>63</v>
+      </c>
+      <c r="Q15">
         <v>61</v>
       </c>
-      <c r="D15">
-        <v>75</v>
-      </c>
-      <c r="E15">
+      <c r="R15">
+        <v>47</v>
+      </c>
+      <c r="S15">
+        <v>80</v>
+      </c>
+      <c r="T15">
+        <v>53</v>
+      </c>
+      <c r="U15">
+        <v>94</v>
+      </c>
+      <c r="V15">
+        <v>50</v>
+      </c>
+      <c r="W15">
+        <v>80</v>
+      </c>
+      <c r="X15">
         <v>68</v>
       </c>
-      <c r="F15">
+      <c r="Y15">
+        <v>69</v>
+      </c>
+      <c r="Z15">
+        <v>128</v>
+      </c>
+      <c r="AA15">
+        <v>102</v>
+      </c>
+      <c r="AB15">
+        <v>89</v>
+      </c>
+      <c r="AC15">
+        <v>56</v>
+      </c>
+      <c r="AD15">
         <v>63</v>
       </c>
-      <c r="G15">
-        <v>88</v>
-      </c>
-      <c r="H15">
-        <v>38</v>
-      </c>
-      <c r="I15">
-        <v>68</v>
-      </c>
-      <c r="J15">
-        <v>24</v>
-      </c>
-      <c r="K15">
-        <v>65</v>
-      </c>
-      <c r="L15">
-        <v>30</v>
-      </c>
-      <c r="M15">
-        <v>46</v>
-      </c>
-      <c r="N15">
-        <v>29</v>
-      </c>
-      <c r="O15">
-        <v>89</v>
-      </c>
-      <c r="P15">
-        <v>50</v>
-      </c>
-      <c r="Q15">
-        <v>45</v>
-      </c>
-      <c r="R15">
-        <v>80</v>
-      </c>
-      <c r="S15">
-        <v>105</v>
-      </c>
-      <c r="T15">
-        <v>77</v>
-      </c>
-      <c r="U15">
-        <v>86</v>
-      </c>
-      <c r="V15">
-        <v>85</v>
-      </c>
-      <c r="W15">
-        <v>57</v>
-      </c>
-      <c r="X15">
-        <v>25</v>
-      </c>
-      <c r="Y15">
-        <v>56</v>
-      </c>
-      <c r="Z15">
-        <v>132</v>
-      </c>
-      <c r="AA15">
-        <v>82</v>
-      </c>
-      <c r="AB15">
-        <v>70</v>
-      </c>
-      <c r="AC15">
-        <v>51</v>
+      <c r="AE15">
+        <v>52</v>
       </c>
       <c r="AO15">
         <f>SUM(Tabell1[[#This Row],[GW1]:[GW38]])</f>
-        <v>1745</v>
+        <v>1969</v>
       </c>
     </row>
     <row r="16" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>60</v>
+        <v>103</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>104</v>
       </c>
       <c r="C16">
+        <v>48</v>
+      </c>
+      <c r="D16">
+        <v>90</v>
+      </c>
+      <c r="E16">
+        <v>89</v>
+      </c>
+      <c r="F16">
+        <v>53</v>
+      </c>
+      <c r="G16">
+        <v>75</v>
+      </c>
+      <c r="H16">
+        <v>32</v>
+      </c>
+      <c r="I16">
+        <v>48</v>
+      </c>
+      <c r="J16">
+        <v>40</v>
+      </c>
+      <c r="K16">
+        <v>65</v>
+      </c>
+      <c r="L16">
+        <v>34</v>
+      </c>
+      <c r="M16">
+        <v>39</v>
+      </c>
+      <c r="N16">
+        <v>22</v>
+      </c>
+      <c r="O16">
+        <v>65</v>
+      </c>
+      <c r="P16">
+        <v>77</v>
+      </c>
+      <c r="Q16">
+        <v>56</v>
+      </c>
+      <c r="R16">
+        <v>47</v>
+      </c>
+      <c r="S16">
+        <v>57</v>
+      </c>
+      <c r="T16">
+        <v>54</v>
+      </c>
+      <c r="U16">
+        <v>75</v>
+      </c>
+      <c r="V16">
+        <v>59</v>
+      </c>
+      <c r="W16">
+        <v>50</v>
+      </c>
+      <c r="X16">
+        <v>31</v>
+      </c>
+      <c r="Y16">
+        <v>62</v>
+      </c>
+      <c r="Z16">
+        <v>133</v>
+      </c>
+      <c r="AA16">
+        <v>84</v>
+      </c>
+      <c r="AB16">
+        <v>70</v>
+      </c>
+      <c r="AC16">
         <v>55</v>
       </c>
-      <c r="D16">
-        <v>33</v>
-      </c>
-      <c r="E16">
-        <v>69</v>
-      </c>
-      <c r="F16">
-        <v>65</v>
-      </c>
-      <c r="G16">
-        <v>66</v>
-      </c>
-      <c r="H16">
-        <v>69</v>
-      </c>
-      <c r="I16">
-        <v>39</v>
-      </c>
-      <c r="J16">
-        <v>52</v>
-      </c>
-      <c r="K16">
-        <v>74</v>
-      </c>
-      <c r="L16">
-        <v>39</v>
-      </c>
-      <c r="M16">
-        <v>54</v>
-      </c>
-      <c r="N16">
-        <v>39</v>
-      </c>
-      <c r="O16">
-        <v>47</v>
-      </c>
-      <c r="P16">
-        <v>68</v>
-      </c>
-      <c r="Q16">
-        <v>59</v>
-      </c>
-      <c r="R16">
-        <v>62</v>
-      </c>
-      <c r="S16">
-        <v>61</v>
-      </c>
-      <c r="T16">
-        <v>55</v>
-      </c>
-      <c r="U16">
-        <v>68</v>
-      </c>
-      <c r="V16">
-        <v>78</v>
-      </c>
-      <c r="W16">
-        <v>57</v>
-      </c>
-      <c r="X16">
-        <v>38</v>
-      </c>
-      <c r="Y16">
-        <v>48</v>
-      </c>
-      <c r="Z16">
-        <v>114</v>
-      </c>
-      <c r="AA16">
-        <v>80</v>
-      </c>
-      <c r="AB16">
-        <v>85</v>
-      </c>
-      <c r="AC16">
-        <v>50</v>
+      <c r="AD16">
+        <v>41</v>
+      </c>
+      <c r="AE16">
+        <v>51</v>
       </c>
       <c r="AO16">
         <f>SUM(Tabell1[[#This Row],[GW1]:[GW38]])</f>
-        <v>1624</v>
+        <v>1702</v>
       </c>
     </row>
     <row r="17" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>83</v>
       </c>
       <c r="C17">
-        <v>72</v>
+        <v>42</v>
       </c>
       <c r="D17">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E17">
-        <v>95</v>
+        <v>68</v>
       </c>
       <c r="F17">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="G17">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="H17">
+        <v>55</v>
+      </c>
+      <c r="I17">
+        <v>37</v>
+      </c>
+      <c r="J17">
+        <v>36</v>
+      </c>
+      <c r="K17">
+        <v>43</v>
+      </c>
+      <c r="L17">
+        <v>32</v>
+      </c>
+      <c r="M17">
+        <v>59</v>
+      </c>
+      <c r="N17">
+        <v>30</v>
+      </c>
+      <c r="O17">
         <v>45</v>
       </c>
-      <c r="I17">
-        <v>42</v>
-      </c>
-      <c r="J17">
+      <c r="P17">
         <v>53</v>
       </c>
-      <c r="K17">
-        <v>69</v>
-      </c>
-      <c r="L17">
-        <v>38</v>
-      </c>
-      <c r="M17">
+      <c r="Q17">
+        <v>53</v>
+      </c>
+      <c r="R17">
+        <v>53</v>
+      </c>
+      <c r="S17">
+        <v>66</v>
+      </c>
+      <c r="T17">
+        <v>60</v>
+      </c>
+      <c r="U17">
+        <v>49</v>
+      </c>
+      <c r="V17">
+        <v>82</v>
+      </c>
+      <c r="W17">
+        <v>73</v>
+      </c>
+      <c r="X17">
+        <v>53</v>
+      </c>
+      <c r="Y17">
+        <v>83</v>
+      </c>
+      <c r="Z17">
+        <v>130</v>
+      </c>
+      <c r="AA17">
+        <v>71</v>
+      </c>
+      <c r="AB17">
+        <v>74</v>
+      </c>
+      <c r="AC17">
+        <v>46</v>
+      </c>
+      <c r="AD17">
         <v>64</v>
       </c>
-      <c r="N17">
-        <v>57</v>
-      </c>
-      <c r="O17">
-        <v>43</v>
-      </c>
-      <c r="P17">
-        <v>92</v>
-      </c>
-      <c r="Q17">
-        <v>59</v>
-      </c>
-      <c r="R17">
-        <v>77</v>
-      </c>
-      <c r="S17">
-        <v>76</v>
-      </c>
-      <c r="T17">
-        <v>70</v>
-      </c>
-      <c r="U17">
-        <v>80</v>
-      </c>
-      <c r="V17">
-        <v>74</v>
-      </c>
-      <c r="W17">
-        <v>52</v>
-      </c>
-      <c r="X17">
-        <v>36</v>
-      </c>
-      <c r="Y17">
-        <v>59</v>
-      </c>
-      <c r="Z17">
-        <v>131</v>
-      </c>
-      <c r="AA17">
-        <v>87</v>
-      </c>
-      <c r="AB17">
-        <v>89</v>
-      </c>
-      <c r="AC17">
-        <v>48</v>
+      <c r="AE17">
+        <v>49</v>
       </c>
       <c r="AO17">
         <f>SUM(Tabell1[[#This Row],[GW1]:[GW38]])</f>
-        <v>1786</v>
+        <v>1685</v>
       </c>
     </row>
     <row r="18" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>94</v>
+      </c>
+      <c r="B18" t="s">
+        <v>95</v>
+      </c>
+      <c r="C18">
+        <v>62</v>
+      </c>
+      <c r="D18">
+        <v>45</v>
+      </c>
+      <c r="E18">
+        <v>38</v>
+      </c>
+      <c r="F18">
+        <v>38</v>
+      </c>
+      <c r="G18">
         <v>35</v>
       </c>
-      <c r="B18" t="s">
-        <v>102</v>
-      </c>
-      <c r="C18">
-        <v>45</v>
-      </c>
-      <c r="D18">
-        <v>73</v>
-      </c>
-      <c r="E18">
-        <v>78</v>
-      </c>
-      <c r="F18">
-        <v>50</v>
-      </c>
-      <c r="G18">
+      <c r="H18">
         <v>62</v>
       </c>
-      <c r="H18">
-        <v>34</v>
-      </c>
       <c r="I18">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="J18">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="K18">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="L18">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="M18">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="N18">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="O18">
         <v>40</v>
       </c>
       <c r="P18">
+        <v>44</v>
+      </c>
+      <c r="Q18">
+        <v>59</v>
+      </c>
+      <c r="R18">
+        <v>43</v>
+      </c>
+      <c r="S18">
+        <v>49</v>
+      </c>
+      <c r="T18">
+        <v>42</v>
+      </c>
+      <c r="U18">
+        <v>56</v>
+      </c>
+      <c r="V18">
+        <v>75</v>
+      </c>
+      <c r="W18">
+        <v>33</v>
+      </c>
+      <c r="X18">
+        <v>39</v>
+      </c>
+      <c r="Y18">
+        <v>64</v>
+      </c>
+      <c r="Z18">
         <v>69</v>
       </c>
-      <c r="Q18">
-        <v>42</v>
-      </c>
-      <c r="R18">
-        <v>27</v>
-      </c>
-      <c r="S18">
-        <v>26</v>
-      </c>
-      <c r="T18">
-        <v>56</v>
-      </c>
-      <c r="U18">
-        <v>102</v>
-      </c>
-      <c r="V18">
-        <v>58</v>
-      </c>
-      <c r="W18">
-        <v>70</v>
-      </c>
-      <c r="X18">
-        <v>41</v>
-      </c>
-      <c r="Y18">
-        <v>58</v>
-      </c>
-      <c r="Z18">
-        <v>106</v>
-      </c>
       <c r="AA18">
-        <v>87</v>
+        <v>57</v>
       </c>
       <c r="AB18">
-        <v>75</v>
+        <v>34</v>
       </c>
       <c r="AC18">
-        <v>48</v>
+        <v>55</v>
+      </c>
+      <c r="AD18">
+        <v>69</v>
+      </c>
+      <c r="AE18">
+        <v>45</v>
       </c>
       <c r="AO18">
         <f>SUM(Tabell1[[#This Row],[GW1]:[GW38]])</f>
-        <v>1487</v>
+        <v>1392</v>
       </c>
     </row>
     <row r="19" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B19" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C19">
+        <v>79</v>
+      </c>
+      <c r="D19">
+        <v>79</v>
+      </c>
+      <c r="E19">
+        <v>73</v>
+      </c>
+      <c r="F19">
+        <v>60</v>
+      </c>
+      <c r="G19">
+        <v>83</v>
+      </c>
+      <c r="H19">
+        <v>35</v>
+      </c>
+      <c r="I19">
+        <v>64</v>
+      </c>
+      <c r="J19">
+        <v>32</v>
+      </c>
+      <c r="K19">
+        <v>60</v>
+      </c>
+      <c r="L19">
+        <v>31</v>
+      </c>
+      <c r="M19">
+        <v>49</v>
+      </c>
+      <c r="N19">
+        <v>45</v>
+      </c>
+      <c r="O19">
+        <v>90</v>
+      </c>
+      <c r="P19">
+        <v>37</v>
+      </c>
+      <c r="Q19">
         <v>68</v>
       </c>
-      <c r="D19">
-        <v>82</v>
-      </c>
-      <c r="E19">
-        <v>66</v>
-      </c>
-      <c r="F19">
-        <v>53</v>
-      </c>
-      <c r="G19">
-        <v>77</v>
-      </c>
-      <c r="H19">
-        <v>42</v>
-      </c>
-      <c r="I19">
-        <v>59</v>
-      </c>
-      <c r="J19">
-        <v>35</v>
-      </c>
-      <c r="K19">
+      <c r="R19">
         <v>48</v>
       </c>
-      <c r="L19">
-        <v>30</v>
-      </c>
-      <c r="M19">
-        <v>35</v>
-      </c>
-      <c r="N19">
-        <v>62</v>
-      </c>
-      <c r="O19">
-        <v>64</v>
-      </c>
-      <c r="P19">
-        <v>76</v>
-      </c>
-      <c r="Q19">
-        <v>39</v>
-      </c>
-      <c r="R19">
-        <v>45</v>
-      </c>
       <c r="S19">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="T19">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="U19">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="V19">
         <v>56</v>
       </c>
       <c r="W19">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="X19">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="Y19">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="Z19">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="AA19">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="AB19">
-        <v>66</v>
+        <v>95</v>
       </c>
       <c r="AC19">
-        <v>48</v>
+        <v>74</v>
+      </c>
+      <c r="AD19">
+        <v>70</v>
+      </c>
+      <c r="AE19">
+        <v>43</v>
       </c>
       <c r="AO19">
         <f>SUM(Tabell1[[#This Row],[GW1]:[GW38]])</f>
-        <v>1607</v>
+        <v>1891</v>
       </c>
     </row>
     <row r="20" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20">
+        <v>70</v>
+      </c>
+      <c r="D20">
+        <v>78</v>
+      </c>
+      <c r="E20">
+        <v>74</v>
+      </c>
+      <c r="F20">
+        <v>60</v>
+      </c>
+      <c r="G20">
+        <v>58</v>
+      </c>
+      <c r="H20">
+        <v>59</v>
+      </c>
+      <c r="I20">
+        <v>46</v>
+      </c>
+      <c r="J20">
+        <v>47</v>
+      </c>
+      <c r="K20">
+        <v>50</v>
+      </c>
+      <c r="L20">
+        <v>55</v>
+      </c>
+      <c r="M20">
+        <v>69</v>
+      </c>
+      <c r="N20">
+        <v>35</v>
+      </c>
+      <c r="O20">
+        <v>51</v>
+      </c>
+      <c r="P20">
+        <v>92</v>
+      </c>
+      <c r="Q20">
+        <v>52</v>
+      </c>
+      <c r="R20">
+        <v>49</v>
+      </c>
+      <c r="S20">
+        <v>104</v>
+      </c>
+      <c r="T20">
         <v>44</v>
       </c>
-      <c r="B20" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20">
-        <v>67</v>
-      </c>
-      <c r="D20">
-        <v>71</v>
-      </c>
-      <c r="E20">
-        <v>64</v>
-      </c>
-      <c r="F20">
-        <v>52</v>
-      </c>
-      <c r="G20">
-        <v>65</v>
-      </c>
-      <c r="H20">
+      <c r="U20">
+        <v>59</v>
+      </c>
+      <c r="V20">
+        <v>55</v>
+      </c>
+      <c r="W20">
         <v>61</v>
       </c>
-      <c r="I20">
-        <v>58</v>
-      </c>
-      <c r="J20">
-        <v>31</v>
-      </c>
-      <c r="K20">
-        <v>31</v>
-      </c>
-      <c r="L20">
-        <v>57</v>
-      </c>
-      <c r="M20">
-        <v>81</v>
-      </c>
-      <c r="N20">
-        <v>54</v>
-      </c>
-      <c r="O20">
-        <v>55</v>
-      </c>
-      <c r="P20">
-        <v>74</v>
-      </c>
-      <c r="Q20">
-        <v>55</v>
-      </c>
-      <c r="R20">
-        <v>70</v>
-      </c>
-      <c r="S20">
-        <v>103</v>
-      </c>
-      <c r="T20">
-        <v>74</v>
-      </c>
-      <c r="U20">
-        <v>73</v>
-      </c>
-      <c r="V20">
-        <v>70</v>
-      </c>
-      <c r="W20">
-        <v>98</v>
-      </c>
       <c r="X20">
+        <v>59</v>
+      </c>
+      <c r="Y20">
+        <v>62</v>
+      </c>
+      <c r="Z20">
+        <v>144</v>
+      </c>
+      <c r="AA20">
+        <v>109</v>
+      </c>
+      <c r="AB20">
+        <v>92</v>
+      </c>
+      <c r="AC20">
         <v>42</v>
       </c>
-      <c r="Y20">
-        <v>56</v>
-      </c>
-      <c r="Z20">
-        <v>114</v>
-      </c>
-      <c r="AA20">
-        <v>99</v>
-      </c>
-      <c r="AB20">
-        <v>80</v>
-      </c>
-      <c r="AC20">
-        <v>46</v>
+      <c r="AD20">
+        <v>49</v>
+      </c>
+      <c r="AE20">
+        <v>43</v>
       </c>
       <c r="AO20">
         <f>SUM(Tabell1[[#This Row],[GW1]:[GW38]])</f>
-        <v>1801</v>
+        <v>1868</v>
       </c>
     </row>
     <row r="21" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B21" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21">
+        <v>76</v>
+      </c>
+      <c r="D21">
+        <v>74</v>
+      </c>
+      <c r="E21">
+        <v>69</v>
+      </c>
+      <c r="F21">
+        <v>56</v>
+      </c>
+      <c r="G21">
+        <v>62</v>
+      </c>
+      <c r="H21">
+        <v>62</v>
+      </c>
+      <c r="I21">
+        <v>49</v>
+      </c>
+      <c r="J21">
+        <v>47</v>
+      </c>
+      <c r="K21">
+        <v>46</v>
+      </c>
+      <c r="L21">
+        <v>42</v>
+      </c>
+      <c r="M21">
+        <v>46</v>
+      </c>
+      <c r="N21">
+        <v>72</v>
+      </c>
+      <c r="O21">
+        <v>49</v>
+      </c>
+      <c r="P21">
+        <v>66</v>
+      </c>
+      <c r="Q21">
+        <v>39</v>
+      </c>
+      <c r="R21">
+        <v>52</v>
+      </c>
+      <c r="S21">
+        <v>69</v>
+      </c>
+      <c r="T21">
+        <v>62</v>
+      </c>
+      <c r="U21">
+        <v>61</v>
+      </c>
+      <c r="V21">
+        <v>63</v>
+      </c>
+      <c r="W21">
         <v>83</v>
       </c>
-      <c r="C21">
-        <v>42</v>
-      </c>
-      <c r="D21">
-        <v>68</v>
-      </c>
-      <c r="E21">
-        <v>68</v>
-      </c>
-      <c r="F21">
-        <v>61</v>
-      </c>
-      <c r="G21">
-        <v>50</v>
-      </c>
-      <c r="H21">
-        <v>55</v>
-      </c>
-      <c r="I21">
-        <v>37</v>
-      </c>
-      <c r="J21">
-        <v>36</v>
-      </c>
-      <c r="K21">
-        <v>43</v>
-      </c>
-      <c r="L21">
-        <v>32</v>
-      </c>
-      <c r="M21">
-        <v>59</v>
-      </c>
-      <c r="N21">
-        <v>30</v>
-      </c>
-      <c r="O21">
-        <v>45</v>
-      </c>
-      <c r="P21">
-        <v>53</v>
-      </c>
-      <c r="Q21">
-        <v>53</v>
-      </c>
-      <c r="R21">
-        <v>53</v>
-      </c>
-      <c r="S21">
-        <v>66</v>
-      </c>
-      <c r="T21">
+      <c r="X21">
+        <v>47</v>
+      </c>
+      <c r="Y21">
+        <v>49</v>
+      </c>
+      <c r="Z21">
+        <v>91</v>
+      </c>
+      <c r="AA21">
+        <v>56</v>
+      </c>
+      <c r="AB21">
         <v>60</v>
-      </c>
-      <c r="U21">
-        <v>49</v>
-      </c>
-      <c r="V21">
-        <v>82</v>
-      </c>
-      <c r="W21">
-        <v>73</v>
-      </c>
-      <c r="X21">
-        <v>53</v>
-      </c>
-      <c r="Y21">
-        <v>83</v>
-      </c>
-      <c r="Z21">
-        <v>130</v>
-      </c>
-      <c r="AA21">
-        <v>71</v>
-      </c>
-      <c r="AB21">
-        <v>74</v>
       </c>
       <c r="AC21">
         <v>46</v>
       </c>
+      <c r="AD21">
+        <v>51</v>
+      </c>
+      <c r="AE21">
+        <v>34</v>
+      </c>
       <c r="AO21">
         <f>SUM(Tabell1[[#This Row],[GW1]:[GW38]])</f>
-        <v>1572</v>
+        <v>1679</v>
       </c>
     </row>
     <row r="22" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="B22" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C22">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D22">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="E22">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F22">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="G22">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="H22">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="I22">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="J22">
         <v>52</v>
       </c>
       <c r="K22">
+        <v>74</v>
+      </c>
+      <c r="L22">
+        <v>39</v>
+      </c>
+      <c r="M22">
+        <v>54</v>
+      </c>
+      <c r="N22">
+        <v>39</v>
+      </c>
+      <c r="O22">
+        <v>47</v>
+      </c>
+      <c r="P22">
+        <v>68</v>
+      </c>
+      <c r="Q22">
+        <v>59</v>
+      </c>
+      <c r="R22">
+        <v>62</v>
+      </c>
+      <c r="S22">
+        <v>61</v>
+      </c>
+      <c r="T22">
         <v>55</v>
       </c>
-      <c r="L22">
-        <v>47</v>
-      </c>
-      <c r="M22">
-        <v>70</v>
-      </c>
-      <c r="N22">
-        <v>72</v>
-      </c>
-      <c r="O22">
-        <v>77</v>
-      </c>
-      <c r="P22">
-        <v>62</v>
-      </c>
-      <c r="Q22">
-        <v>42</v>
-      </c>
-      <c r="R22">
-        <v>51</v>
-      </c>
-      <c r="S22">
-        <v>90</v>
-      </c>
-      <c r="T22">
-        <v>72</v>
-      </c>
       <c r="U22">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="V22">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="W22">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="X22">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="Y22">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="Z22">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="AA22">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="AB22">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="AC22">
-        <v>46</v>
+        <v>50</v>
+      </c>
+      <c r="AD22">
+        <v>54</v>
+      </c>
+      <c r="AE22">
+        <v>33</v>
       </c>
       <c r="AO22">
         <f>SUM(Tabell1[[#This Row],[GW1]:[GW38]])</f>
-        <v>1741</v>
+        <v>1711</v>
       </c>
     </row>
     <row r="23" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>64</v>
       </c>
       <c r="B23" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C23">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="D23">
-        <v>78</v>
+        <v>98</v>
       </c>
       <c r="E23">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="F23">
+        <v>59</v>
+      </c>
+      <c r="G23">
+        <v>56</v>
+      </c>
+      <c r="H23">
+        <v>57</v>
+      </c>
+      <c r="I23">
+        <v>55</v>
+      </c>
+      <c r="J23">
+        <v>56</v>
+      </c>
+      <c r="K23">
+        <v>67</v>
+      </c>
+      <c r="L23">
+        <v>48</v>
+      </c>
+      <c r="M23">
+        <v>31</v>
+      </c>
+      <c r="N23">
+        <v>52</v>
+      </c>
+      <c r="O23">
+        <v>64</v>
+      </c>
+      <c r="P23">
+        <v>62</v>
+      </c>
+      <c r="Q23">
+        <v>49</v>
+      </c>
+      <c r="R23">
+        <v>54</v>
+      </c>
+      <c r="S23">
+        <v>100</v>
+      </c>
+      <c r="T23">
+        <v>62</v>
+      </c>
+      <c r="U23">
+        <v>87</v>
+      </c>
+      <c r="V23">
+        <v>49</v>
+      </c>
+      <c r="W23">
         <v>60</v>
       </c>
-      <c r="G23">
-        <v>58</v>
-      </c>
-      <c r="H23">
-        <v>59</v>
-      </c>
-      <c r="I23">
-        <v>46</v>
-      </c>
-      <c r="J23">
-        <v>47</v>
-      </c>
-      <c r="K23">
+      <c r="X23">
         <v>50</v>
       </c>
-      <c r="L23">
-        <v>55</v>
-      </c>
-      <c r="M23">
-        <v>69</v>
-      </c>
-      <c r="N23">
-        <v>35</v>
-      </c>
-      <c r="O23">
-        <v>51</v>
-      </c>
-      <c r="P23">
-        <v>92</v>
-      </c>
-      <c r="Q23">
-        <v>52</v>
-      </c>
-      <c r="R23">
-        <v>49</v>
-      </c>
-      <c r="S23">
-        <v>104</v>
-      </c>
-      <c r="T23">
-        <v>44</v>
-      </c>
-      <c r="U23">
-        <v>59</v>
-      </c>
-      <c r="V23">
-        <v>55</v>
-      </c>
-      <c r="W23">
-        <v>61</v>
-      </c>
-      <c r="X23">
-        <v>59</v>
-      </c>
       <c r="Y23">
-        <v>62</v>
+        <v>87</v>
       </c>
       <c r="Z23">
-        <v>144</v>
+        <v>93</v>
       </c>
       <c r="AA23">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="AB23">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="AC23">
-        <v>42</v>
+        <v>85</v>
+      </c>
+      <c r="AD23">
+        <v>60</v>
+      </c>
+      <c r="AE23">
+        <v>32</v>
       </c>
       <c r="AO23">
         <f>SUM(Tabell1[[#This Row],[GW1]:[GW38]])</f>
-        <v>1776</v>
+        <v>1887</v>
       </c>
     </row>
     <row r="24" spans="1:41" x14ac:dyDescent="0.25">
@@ -5208,290 +5334,314 @@
         <v>71</v>
       </c>
       <c r="AC24">
-        <v>40</v>
+        <v>43</v>
+      </c>
+      <c r="AD24">
+        <v>59</v>
+      </c>
+      <c r="AE24">
+        <v>27</v>
       </c>
       <c r="AO24">
         <f>SUM(Tabell1[[#This Row],[GW1]:[GW38]])</f>
-        <v>1548</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="25" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>98</v>
+        <v>52</v>
       </c>
       <c r="B25" t="s">
-        <v>99</v>
+        <v>53</v>
       </c>
       <c r="C25">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D25">
+        <v>62</v>
+      </c>
+      <c r="E25">
+        <v>71</v>
+      </c>
+      <c r="F25">
+        <v>48</v>
+      </c>
+      <c r="G25">
+        <v>61</v>
+      </c>
+      <c r="H25">
+        <v>51</v>
+      </c>
+      <c r="I25">
+        <v>23</v>
+      </c>
+      <c r="J25">
+        <v>52</v>
+      </c>
+      <c r="K25">
+        <v>55</v>
+      </c>
+      <c r="L25">
+        <v>47</v>
+      </c>
+      <c r="M25">
+        <v>70</v>
+      </c>
+      <c r="N25">
+        <v>72</v>
+      </c>
+      <c r="O25">
+        <v>77</v>
+      </c>
+      <c r="P25">
+        <v>62</v>
+      </c>
+      <c r="Q25">
+        <v>42</v>
+      </c>
+      <c r="R25">
+        <v>51</v>
+      </c>
+      <c r="S25">
+        <v>90</v>
+      </c>
+      <c r="T25">
+        <v>72</v>
+      </c>
+      <c r="U25">
+        <v>79</v>
+      </c>
+      <c r="V25">
+        <v>76</v>
+      </c>
+      <c r="W25">
         <v>78</v>
       </c>
-      <c r="E25">
-        <v>84</v>
-      </c>
-      <c r="F25">
-        <v>56</v>
-      </c>
-      <c r="G25">
-        <v>63</v>
-      </c>
-      <c r="H25">
-        <v>34</v>
-      </c>
-      <c r="I25">
-        <v>54</v>
-      </c>
-      <c r="J25">
-        <v>25</v>
-      </c>
-      <c r="K25">
-        <v>68</v>
-      </c>
-      <c r="L25">
-        <v>38</v>
-      </c>
-      <c r="M25">
-        <v>56</v>
-      </c>
-      <c r="N25">
-        <v>45</v>
-      </c>
-      <c r="O25">
-        <v>49</v>
-      </c>
-      <c r="P25">
-        <v>44</v>
-      </c>
-      <c r="Q25">
-        <v>69</v>
-      </c>
-      <c r="R25">
-        <v>43</v>
-      </c>
-      <c r="S25">
-        <v>54</v>
-      </c>
-      <c r="T25">
-        <v>43</v>
-      </c>
-      <c r="U25">
-        <v>48</v>
-      </c>
-      <c r="V25">
+      <c r="X25">
+        <v>66</v>
+      </c>
+      <c r="Y25">
+        <v>59</v>
+      </c>
+      <c r="Z25">
+        <v>124</v>
+      </c>
+      <c r="AA25">
+        <v>89</v>
+      </c>
+      <c r="AB25">
+        <v>61</v>
+      </c>
+      <c r="AC25">
+        <v>52</v>
+      </c>
+      <c r="AD25">
         <v>55</v>
       </c>
-      <c r="W25">
-        <v>61</v>
-      </c>
-      <c r="X25">
-        <v>41</v>
-      </c>
-      <c r="Y25">
-        <v>62</v>
-      </c>
-      <c r="Z25">
-        <v>103</v>
-      </c>
-      <c r="AA25">
-        <v>64</v>
-      </c>
-      <c r="AB25">
-        <v>74</v>
-      </c>
-      <c r="AC25">
-        <v>39</v>
+      <c r="AE25">
+        <v>26</v>
       </c>
       <c r="AO25">
         <f>SUM(Tabell1[[#This Row],[GW1]:[GW38]])</f>
-        <v>1504</v>
+        <v>1828</v>
       </c>
     </row>
     <row r="26" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26">
+        <v>61</v>
+      </c>
+      <c r="D26">
+        <v>75</v>
+      </c>
+      <c r="E26">
+        <v>68</v>
+      </c>
+      <c r="F26">
+        <v>63</v>
+      </c>
+      <c r="G26">
+        <v>88</v>
+      </c>
+      <c r="H26">
+        <v>38</v>
+      </c>
+      <c r="I26">
+        <v>68</v>
+      </c>
+      <c r="J26">
+        <v>24</v>
+      </c>
+      <c r="K26">
+        <v>65</v>
+      </c>
+      <c r="L26">
+        <v>30</v>
+      </c>
+      <c r="M26">
+        <v>46</v>
+      </c>
+      <c r="N26">
+        <v>29</v>
+      </c>
+      <c r="O26">
+        <v>89</v>
+      </c>
+      <c r="P26">
+        <v>50</v>
+      </c>
+      <c r="Q26">
+        <v>45</v>
+      </c>
+      <c r="R26">
+        <v>80</v>
+      </c>
+      <c r="S26">
+        <v>105</v>
+      </c>
+      <c r="T26">
+        <v>77</v>
+      </c>
+      <c r="U26">
         <v>86</v>
       </c>
-      <c r="B26" t="s">
-        <v>59</v>
-      </c>
-      <c r="C26">
-        <v>81</v>
-      </c>
-      <c r="D26">
-        <v>71</v>
-      </c>
-      <c r="E26">
+      <c r="V26">
         <v>85</v>
       </c>
-      <c r="F26">
-        <v>48</v>
-      </c>
-      <c r="G26">
-        <v>61</v>
-      </c>
-      <c r="H26">
-        <v>68</v>
-      </c>
-      <c r="I26">
-        <v>71</v>
-      </c>
-      <c r="J26">
-        <v>48</v>
-      </c>
-      <c r="K26">
+      <c r="W26">
+        <v>57</v>
+      </c>
+      <c r="X26">
+        <v>25</v>
+      </c>
+      <c r="Y26">
+        <v>56</v>
+      </c>
+      <c r="Z26">
+        <v>132</v>
+      </c>
+      <c r="AA26">
+        <v>82</v>
+      </c>
+      <c r="AB26">
         <v>70</v>
       </c>
-      <c r="L26">
-        <v>38</v>
-      </c>
-      <c r="M26">
-        <v>66</v>
-      </c>
-      <c r="N26">
-        <v>42</v>
-      </c>
-      <c r="O26">
-        <v>62</v>
-      </c>
-      <c r="P26">
-        <v>55</v>
-      </c>
-      <c r="Q26">
-        <v>52</v>
-      </c>
-      <c r="R26">
-        <v>82</v>
-      </c>
-      <c r="S26">
-        <v>53</v>
-      </c>
-      <c r="T26">
-        <v>61</v>
-      </c>
-      <c r="U26">
-        <v>87</v>
-      </c>
-      <c r="V26">
-        <v>52</v>
-      </c>
-      <c r="W26">
-        <v>91</v>
-      </c>
-      <c r="X26">
-        <v>47</v>
-      </c>
-      <c r="Y26">
-        <v>73</v>
-      </c>
-      <c r="Z26">
-        <v>136</v>
-      </c>
-      <c r="AA26">
-        <v>91</v>
-      </c>
-      <c r="AB26">
-        <v>79</v>
-      </c>
       <c r="AC26">
-        <v>35</v>
+        <v>50</v>
+      </c>
+      <c r="AD26">
+        <v>58</v>
+      </c>
+      <c r="AE26">
+        <v>15</v>
       </c>
       <c r="AO26">
         <f>SUM(Tabell1[[#This Row],[GW1]:[GW38]])</f>
-        <v>1805</v>
+        <v>1817</v>
       </c>
     </row>
     <row r="27" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>77</v>
+        <v>35</v>
       </c>
       <c r="B27" t="s">
+        <v>102</v>
+      </c>
+      <c r="C27">
+        <v>45</v>
+      </c>
+      <c r="D27">
+        <v>73</v>
+      </c>
+      <c r="E27">
         <v>78</v>
       </c>
-      <c r="C27">
-        <v>76</v>
-      </c>
-      <c r="D27">
-        <v>74</v>
-      </c>
-      <c r="E27">
-        <v>69</v>
-      </c>
       <c r="F27">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="G27">
         <v>62</v>
       </c>
       <c r="H27">
-        <v>62</v>
+        <v>34</v>
       </c>
       <c r="I27">
         <v>49</v>
       </c>
       <c r="J27">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="K27">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="L27">
+        <v>39</v>
+      </c>
+      <c r="M27">
+        <v>38</v>
+      </c>
+      <c r="N27">
         <v>42</v>
       </c>
-      <c r="M27">
-        <v>46</v>
-      </c>
-      <c r="N27">
-        <v>72</v>
-      </c>
       <c r="O27">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="P27">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="Q27">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="R27">
+        <v>27</v>
+      </c>
+      <c r="S27">
+        <v>26</v>
+      </c>
+      <c r="T27">
+        <v>56</v>
+      </c>
+      <c r="U27">
+        <v>102</v>
+      </c>
+      <c r="V27">
+        <v>58</v>
+      </c>
+      <c r="W27">
+        <v>70</v>
+      </c>
+      <c r="X27">
+        <v>41</v>
+      </c>
+      <c r="Y27">
+        <v>58</v>
+      </c>
+      <c r="Z27">
+        <v>106</v>
+      </c>
+      <c r="AA27">
+        <v>87</v>
+      </c>
+      <c r="AB27">
+        <v>75</v>
+      </c>
+      <c r="AC27">
         <v>52</v>
       </c>
-      <c r="S27">
-        <v>69</v>
-      </c>
-      <c r="T27">
-        <v>62</v>
-      </c>
-      <c r="U27">
-        <v>61</v>
-      </c>
-      <c r="V27">
+      <c r="AD27">
         <v>63</v>
       </c>
-      <c r="W27">
-        <v>83</v>
-      </c>
-      <c r="X27">
-        <v>47</v>
-      </c>
-      <c r="Y27">
-        <v>49</v>
-      </c>
-      <c r="Z27">
-        <v>91</v>
-      </c>
-      <c r="AA27">
-        <v>56</v>
-      </c>
-      <c r="AB27">
-        <v>60</v>
-      </c>
-      <c r="AC27">
-        <v>35</v>
+      <c r="AE27">
+        <v>11</v>
       </c>
       <c r="AO27">
         <f>SUM(Tabell1[[#This Row],[GW1]:[GW38]])</f>
-        <v>1583</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="30" spans="1:41" x14ac:dyDescent="0.25">

</xml_diff>